<commit_message>
saved 243 db lca excel
</commit_message>
<xml_diff>
--- a/analyses/pronovo-2019/cyano-fungi-workup.xlsx
+++ b/analyses/pronovo-2019/cyano-fungi-workup.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/pronovo-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724FE709-56DF-D640-A99F-7DB3698EA87C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078A240E-ABDF-1C41-8297-59FD6895A5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
   </bookViews>
   <sheets>
     <sheet name="cyano dno + db peps tryptic" sheetId="1" r:id="rId1"/>
     <sheet name="fungi dno + db peps tryptic" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
   <si>
     <t>LASGLDAVTK</t>
   </si>
@@ -173,6 +175,123 @@
   </si>
   <si>
     <t>combined db fungi</t>
+  </si>
+  <si>
+    <t>combined lca db fungi</t>
+  </si>
+  <si>
+    <t>Phialophora americana</t>
+  </si>
+  <si>
+    <t>Pezizomycotina</t>
+  </si>
+  <si>
+    <t>Trichoderma gamsii</t>
+  </si>
+  <si>
+    <t>Scedosporium boydii</t>
+  </si>
+  <si>
+    <t>Endocarpon pusillum</t>
+  </si>
+  <si>
+    <t>Fungi</t>
+  </si>
+  <si>
+    <t>Rhodotorula</t>
+  </si>
+  <si>
+    <t>Puccinia sorghi</t>
+  </si>
+  <si>
+    <t>Colletotrichum higginsianum</t>
+  </si>
+  <si>
+    <t>Dikarya</t>
+  </si>
+  <si>
+    <t>Mucor circinelloides f. circinelloides</t>
+  </si>
+  <si>
+    <t>Mortierella elongata</t>
+  </si>
+  <si>
+    <t>Colletotrichum</t>
+  </si>
+  <si>
+    <t>Fonsecaea multimorphosa</t>
+  </si>
+  <si>
+    <t>ALQSDSALK</t>
+  </si>
+  <si>
+    <t>AGPFGQLFR</t>
+  </si>
+  <si>
+    <t>AGPFGQLFRPD</t>
+  </si>
+  <si>
+    <t>TLLDSVVEGK</t>
+  </si>
+  <si>
+    <t>PGQLNSDLR</t>
+  </si>
+  <si>
+    <t>AAALQFTR</t>
+  </si>
+  <si>
+    <t>AGPFGQLFRP</t>
+  </si>
+  <si>
+    <t>VVTLLVNK</t>
+  </si>
+  <si>
+    <t>QLLLGFSK</t>
+  </si>
+  <si>
+    <t>SQEATLEK</t>
+  </si>
+  <si>
+    <t>VSDTVVEPYNA</t>
+  </si>
+  <si>
+    <t>FYTTELDK</t>
+  </si>
+  <si>
+    <t>LAFEPSNLK</t>
+  </si>
+  <si>
+    <t>DSELCLR</t>
+  </si>
+  <si>
+    <t>LTNTGSVK</t>
+  </si>
+  <si>
+    <t>VSDTVVEPYNATLSVHQLVEN</t>
+  </si>
+  <si>
+    <t>AGPFGQLF</t>
+  </si>
+  <si>
+    <t>QASLPLDR</t>
+  </si>
+  <si>
+    <t>GLSVGDGR</t>
+  </si>
+  <si>
+    <t>VSHQVPR</t>
+  </si>
+  <si>
+    <t>TSGWFSK</t>
+  </si>
+  <si>
+    <t>Laccaria amethystina</t>
+  </si>
+  <si>
+    <t>Suillus luteus</t>
+  </si>
+  <si>
+    <t>Stachybotrys</t>
   </si>
 </sst>
 </file>
@@ -537,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F8545A-13E4-384E-A901-CD63BD0C8560}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -774,10 +893,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39D6E-ADCE-C54E-86E3-C5932C98575B}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -798,7 +917,7 @@
     <col min="14" max="14" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -840,6 +959,201 @@
       </c>
       <c r="N1" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" t="s">
+        <v>80</v>
+      </c>
+      <c r="J3" t="s">
+        <v>66</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I4" t="s">
+        <v>81</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" t="s">
+        <v>82</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>67</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+      <c r="O10" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+      <c r="O15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>76</v>
+      </c>
+      <c r="O16" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>78</v>
+      </c>
+      <c r="O18" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>79</v>
+      </c>
+      <c r="O19" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="8:15" x14ac:dyDescent="0.2">
+      <c r="O25" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added xlxs versions of db lca
</commit_message>
<xml_diff>
--- a/analyses/pronovo-2019/cyano-fungi-workup.xlsx
+++ b/analyses/pronovo-2019/cyano-fungi-workup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/pronovo-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078A240E-ABDF-1C41-8297-59FD6895A5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B228A9D-0699-BA42-9B4B-7CDAE9385034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="454">
   <si>
     <t>LASGLDAVTK</t>
   </si>
@@ -292,6 +292,1110 @@
   </si>
   <si>
     <t>Stachybotrys</t>
+  </si>
+  <si>
+    <t>AVFPSLVGRP</t>
+  </si>
+  <si>
+    <t>TTGLVLDSGDGVTH</t>
+  </si>
+  <si>
+    <t>EVSSLLVR</t>
+  </si>
+  <si>
+    <t>LGSLSLPR</t>
+  </si>
+  <si>
+    <t>Trichophyton concentricum</t>
+  </si>
+  <si>
+    <t>Ascomycota</t>
+  </si>
+  <si>
+    <t>Hydnomerulius pinastri</t>
+  </si>
+  <si>
+    <t>Schizophyllum commune</t>
+  </si>
+  <si>
+    <t>VAAANRPR</t>
+  </si>
+  <si>
+    <t>Rachicladosporium antarcticum</t>
+  </si>
+  <si>
+    <t>SSLSELNEK</t>
+  </si>
+  <si>
+    <t>Aspergillus udagawae</t>
+  </si>
+  <si>
+    <t>combined lca dno fungi</t>
+  </si>
+  <si>
+    <t>RPTGEQK</t>
+  </si>
+  <si>
+    <t>VVTVSLPR</t>
+  </si>
+  <si>
+    <t>WLSLWNK</t>
+  </si>
+  <si>
+    <t>YSQSSPAR</t>
+  </si>
+  <si>
+    <t>SPLDLQLR</t>
+  </si>
+  <si>
+    <t>DVALWTAK</t>
+  </si>
+  <si>
+    <t>GNSVVLSR</t>
+  </si>
+  <si>
+    <t>EPVLDVER</t>
+  </si>
+  <si>
+    <t>LMEFHDK</t>
+  </si>
+  <si>
+    <t>TYMEAPK</t>
+  </si>
+  <si>
+    <t>WTDEDELR</t>
+  </si>
+  <si>
+    <t>LGTVGGPK</t>
+  </si>
+  <si>
+    <t>TVSQLGVK</t>
+  </si>
+  <si>
+    <t>LQWTVPK</t>
+  </si>
+  <si>
+    <t>LLLHSENK</t>
+  </si>
+  <si>
+    <t>LLTHGMDK</t>
+  </si>
+  <si>
+    <t>LDHEAFK</t>
+  </si>
+  <si>
+    <t>LQFMHSR</t>
+  </si>
+  <si>
+    <t>VMLMLPK</t>
+  </si>
+  <si>
+    <t>DPPGVHR</t>
+  </si>
+  <si>
+    <t>LAFMGDK</t>
+  </si>
+  <si>
+    <t>NELNWWR</t>
+  </si>
+  <si>
+    <t>GFVMGPR</t>
+  </si>
+  <si>
+    <t>TPTKPSPK</t>
+  </si>
+  <si>
+    <t>WFMGLVK</t>
+  </si>
+  <si>
+    <t>SEVLYVR</t>
+  </si>
+  <si>
+    <t>Gloeophyllum trabeum</t>
+  </si>
+  <si>
+    <t>Phellinus noxius</t>
+  </si>
+  <si>
+    <t>Trichoderma</t>
+  </si>
+  <si>
+    <t>Polytolypa hystricis</t>
+  </si>
+  <si>
+    <t>Ogataea polymorpha</t>
+  </si>
+  <si>
+    <t>Chaetomium thermophilum var. thermophilum</t>
+  </si>
+  <si>
+    <t>Fibularhizoctonia</t>
+  </si>
+  <si>
+    <t>Rozella allomycis</t>
+  </si>
+  <si>
+    <t>Eurotiales</t>
+  </si>
+  <si>
+    <t>Verruconis gallopava</t>
+  </si>
+  <si>
+    <t>Diplocarpon rosae</t>
+  </si>
+  <si>
+    <t>Saccharomycetaceae</t>
+  </si>
+  <si>
+    <t>Gonapodya prolifera</t>
+  </si>
+  <si>
+    <t>Amphiamblys</t>
+  </si>
+  <si>
+    <t>Macrophomina phaseolina</t>
+  </si>
+  <si>
+    <t>Penicillium camemberti</t>
+  </si>
+  <si>
+    <t>Agaricomycetes</t>
+  </si>
+  <si>
+    <t>Hanseniaspora opuntiae</t>
+  </si>
+  <si>
+    <t>Rhizoctonia solani</t>
+  </si>
+  <si>
+    <t>Kazachstania africana</t>
+  </si>
+  <si>
+    <t>Aspergillus wentii</t>
+  </si>
+  <si>
+    <t>Trichoderma parareesei</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps australis</t>
+  </si>
+  <si>
+    <t>Leucosporidium creatinivorum</t>
+  </si>
+  <si>
+    <t>Verticillium</t>
+  </si>
+  <si>
+    <t>DPLEAVSK</t>
+  </si>
+  <si>
+    <t>EEYLFPR</t>
+  </si>
+  <si>
+    <t>MALEWVAK</t>
+  </si>
+  <si>
+    <t>AVSYETK</t>
+  </si>
+  <si>
+    <t>LVWLHYR</t>
+  </si>
+  <si>
+    <t>WCSVEWK</t>
+  </si>
+  <si>
+    <t>ELVSEDLR</t>
+  </si>
+  <si>
+    <t>TELLWLSR</t>
+  </si>
+  <si>
+    <t>TFWLCPR</t>
+  </si>
+  <si>
+    <t>TVAMWR</t>
+  </si>
+  <si>
+    <t>TNTEVYR</t>
+  </si>
+  <si>
+    <t>AVQMRPR</t>
+  </si>
+  <si>
+    <t>QPGLVNK</t>
+  </si>
+  <si>
+    <t>TLFLDVNK</t>
+  </si>
+  <si>
+    <t>ALQSTPQQK</t>
+  </si>
+  <si>
+    <t>MAMRPLK</t>
+  </si>
+  <si>
+    <t>DEATSVLK</t>
+  </si>
+  <si>
+    <t>HLTPVPPK</t>
+  </si>
+  <si>
+    <t>LDMNVGK</t>
+  </si>
+  <si>
+    <t>AMYAYAK</t>
+  </si>
+  <si>
+    <t>ANYVQNR</t>
+  </si>
+  <si>
+    <t>Magnaporthaceae</t>
+  </si>
+  <si>
+    <t>Elsinoe</t>
+  </si>
+  <si>
+    <t>Herpotrichiellaceae</t>
+  </si>
+  <si>
+    <t>Tuber melanosporum</t>
+  </si>
+  <si>
+    <t>Rhodotorula toruloides</t>
+  </si>
+  <si>
+    <t>Paraphaeosphaeria sporulosa</t>
+  </si>
+  <si>
+    <t>Sporothrix insectorum</t>
+  </si>
+  <si>
+    <t>Hypocreales</t>
+  </si>
+  <si>
+    <t>Gaeumannomyces tritici</t>
+  </si>
+  <si>
+    <t>Paracoccidioides</t>
+  </si>
+  <si>
+    <t>Pseudogymnoascus</t>
+  </si>
+  <si>
+    <t>Penicillium occitanis</t>
+  </si>
+  <si>
+    <t>Trametes pubescens</t>
+  </si>
+  <si>
+    <t>Sordariomycetes</t>
+  </si>
+  <si>
+    <t>[Candida] auris</t>
+  </si>
+  <si>
+    <t>FLNWYFK</t>
+  </si>
+  <si>
+    <t>FSLHLLSK</t>
+  </si>
+  <si>
+    <t>GSNLDLLSR</t>
+  </si>
+  <si>
+    <t>AVFGGAQR</t>
+  </si>
+  <si>
+    <t>MLWSEYR</t>
+  </si>
+  <si>
+    <t>DMSPFDK</t>
+  </si>
+  <si>
+    <t>FHVLALR</t>
+  </si>
+  <si>
+    <t>DPMLSPR</t>
+  </si>
+  <si>
+    <t>AHWYSK</t>
+  </si>
+  <si>
+    <t>SGPPSSYR</t>
+  </si>
+  <si>
+    <t>EVTNPVR</t>
+  </si>
+  <si>
+    <t>TVMMNLAK</t>
+  </si>
+  <si>
+    <t>Kazachstania saulgeensis</t>
+  </si>
+  <si>
+    <t>Neocallimastix californiae</t>
+  </si>
+  <si>
+    <t>Serendipita indica</t>
+  </si>
+  <si>
+    <t>Clonostachys rosea</t>
+  </si>
+  <si>
+    <t>Fusarium</t>
+  </si>
+  <si>
+    <t>Zymoseptoria brevis</t>
+  </si>
+  <si>
+    <t>Phialocephala subalpina</t>
+  </si>
+  <si>
+    <t>Mycena chlorophos</t>
+  </si>
+  <si>
+    <t>Malassezia pachydermatis</t>
+  </si>
+  <si>
+    <t>Stagonospora</t>
+  </si>
+  <si>
+    <t>SMVTTLSR</t>
+  </si>
+  <si>
+    <t>AMTDMLK</t>
+  </si>
+  <si>
+    <t>FSEACMLK</t>
+  </si>
+  <si>
+    <t>NWTMMK</t>
+  </si>
+  <si>
+    <t>TDGPQNK</t>
+  </si>
+  <si>
+    <t>AATTSAPR</t>
+  </si>
+  <si>
+    <t>EVSNWLR</t>
+  </si>
+  <si>
+    <t>YDVLDLSR</t>
+  </si>
+  <si>
+    <t>AAQEAEEER</t>
+  </si>
+  <si>
+    <t>ENLEVLLSK</t>
+  </si>
+  <si>
+    <t>LSEEPDVK</t>
+  </si>
+  <si>
+    <t>TEHAEPK</t>
+  </si>
+  <si>
+    <t>TLMQYYK</t>
+  </si>
+  <si>
+    <t>AEELMNQR</t>
+  </si>
+  <si>
+    <t>ASTQQNK</t>
+  </si>
+  <si>
+    <t>EEQWSPR</t>
+  </si>
+  <si>
+    <t>NQEWLSK</t>
+  </si>
+  <si>
+    <t>ALQACCK</t>
+  </si>
+  <si>
+    <t>WFNQYK</t>
+  </si>
+  <si>
+    <t>Ganoderma sinense</t>
+  </si>
+  <si>
+    <t>Lodderomyces elongisporus</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces cryophilus</t>
+  </si>
+  <si>
+    <t>Kwoniella</t>
+  </si>
+  <si>
+    <t>Fusarium langsethiae</t>
+  </si>
+  <si>
+    <t>Penicillium oxalicum</t>
+  </si>
+  <si>
+    <t>Aspergillus</t>
+  </si>
+  <si>
+    <t>Pisolithus tinctorius</t>
+  </si>
+  <si>
+    <t>Diaporthe helianthi</t>
+  </si>
+  <si>
+    <t>Thielavia terrestris</t>
+  </si>
+  <si>
+    <t>Naumovozyma castellii</t>
+  </si>
+  <si>
+    <t>Exophiala xenobiotica</t>
+  </si>
+  <si>
+    <t>Amanita thiersii</t>
+  </si>
+  <si>
+    <t>Penicillium solitum</t>
+  </si>
+  <si>
+    <t>Sclerotinia borealis</t>
+  </si>
+  <si>
+    <t>Pezoloma ericae</t>
+  </si>
+  <si>
+    <t>LFDLVEQK</t>
+  </si>
+  <si>
+    <t>WVEDDVK</t>
+  </si>
+  <si>
+    <t>NVYDEVSK</t>
+  </si>
+  <si>
+    <t>TDDEEFK</t>
+  </si>
+  <si>
+    <t>TCTAEELK</t>
+  </si>
+  <si>
+    <t>EEELEMPK</t>
+  </si>
+  <si>
+    <t>LLYEEANK</t>
+  </si>
+  <si>
+    <t>LVCDDQR</t>
+  </si>
+  <si>
+    <t>SLAMNER</t>
+  </si>
+  <si>
+    <t>TFQWEAK</t>
+  </si>
+  <si>
+    <t>EAGPLNLR</t>
+  </si>
+  <si>
+    <t>SPGDYTK</t>
+  </si>
+  <si>
+    <t>MVVMEGK</t>
+  </si>
+  <si>
+    <t>NAYDTSHR</t>
+  </si>
+  <si>
+    <t>HMFDGLK</t>
+  </si>
+  <si>
+    <t>LVLSWWK</t>
+  </si>
+  <si>
+    <t>VLNFDNK</t>
+  </si>
+  <si>
+    <t>FFQSGPK</t>
+  </si>
+  <si>
+    <t>MESVHEK</t>
+  </si>
+  <si>
+    <t>FVTTAFK</t>
+  </si>
+  <si>
+    <t>SVVCQAK</t>
+  </si>
+  <si>
+    <t>TVAFFPR</t>
+  </si>
+  <si>
+    <t>DEEFNAR</t>
+  </si>
+  <si>
+    <t>SPATSSAPK</t>
+  </si>
+  <si>
+    <t>AAGGLGKPGK</t>
+  </si>
+  <si>
+    <t>MMLVGPK</t>
+  </si>
+  <si>
+    <t>SYEETLQQK</t>
+  </si>
+  <si>
+    <t>TTDLGEPK</t>
+  </si>
+  <si>
+    <t>TGSLEAYK</t>
+  </si>
+  <si>
+    <t>LCDVLGNK</t>
+  </si>
+  <si>
+    <t>YLNMDPR</t>
+  </si>
+  <si>
+    <t>LNNVEVDVK</t>
+  </si>
+  <si>
+    <t>NQPSFPK</t>
+  </si>
+  <si>
+    <t>YVDWEFK</t>
+  </si>
+  <si>
+    <t>MHSGRPR</t>
+  </si>
+  <si>
+    <t>AMGVPVPR</t>
+  </si>
+  <si>
+    <t>SVNCSLR</t>
+  </si>
+  <si>
+    <t>MNDFMVK</t>
+  </si>
+  <si>
+    <t>NFPQAMK</t>
+  </si>
+  <si>
+    <t>MCLPTPR</t>
+  </si>
+  <si>
+    <t>TELPSMK</t>
+  </si>
+  <si>
+    <t>DCLVGPK</t>
+  </si>
+  <si>
+    <t>GLLYYHK</t>
+  </si>
+  <si>
+    <t>QVGMEQR</t>
+  </si>
+  <si>
+    <t>TVVPALLR</t>
+  </si>
+  <si>
+    <t>WQQPMK</t>
+  </si>
+  <si>
+    <t>AETPPNK</t>
+  </si>
+  <si>
+    <t>EATDLLPK</t>
+  </si>
+  <si>
+    <t>GPFQPPR</t>
+  </si>
+  <si>
+    <t>LWHAEAMK</t>
+  </si>
+  <si>
+    <t>DFYAAHK</t>
+  </si>
+  <si>
+    <t>NNAPVDK</t>
+  </si>
+  <si>
+    <t>TGHCPLK</t>
+  </si>
+  <si>
+    <t>LCGHSYK</t>
+  </si>
+  <si>
+    <t>RPCSNK</t>
+  </si>
+  <si>
+    <t>AFELCLTR</t>
+  </si>
+  <si>
+    <t>MSLPDNGR</t>
+  </si>
+  <si>
+    <t>DPTVNPK</t>
+  </si>
+  <si>
+    <t>YAMDTFK</t>
+  </si>
+  <si>
+    <t>LEDPMVK</t>
+  </si>
+  <si>
+    <t>LSVNCPR</t>
+  </si>
+  <si>
+    <t>MGLYTMR</t>
+  </si>
+  <si>
+    <t>QDTGGSVR</t>
+  </si>
+  <si>
+    <t>TEAYSSAK</t>
+  </si>
+  <si>
+    <t>TASSVLWK</t>
+  </si>
+  <si>
+    <t>WMLWNK</t>
+  </si>
+  <si>
+    <t>GYPMLGK</t>
+  </si>
+  <si>
+    <t>Wickerhamomyces ciferrii</t>
+  </si>
+  <si>
+    <t>[Candida] pseudohaemulonis</t>
+  </si>
+  <si>
+    <t>[Candida] intermedia</t>
+  </si>
+  <si>
+    <t>Saitoella complicata</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces japonicus</t>
+  </si>
+  <si>
+    <t>Nematocida parisii</t>
+  </si>
+  <si>
+    <t>Sporothrix brasiliensis</t>
+  </si>
+  <si>
+    <t>Tilletiaria anomala</t>
+  </si>
+  <si>
+    <t>Penicillium</t>
+  </si>
+  <si>
+    <t>Coccidioides immitis</t>
+  </si>
+  <si>
+    <t>Lobosporangium transversale</t>
+  </si>
+  <si>
+    <t>Clohesyomyces aquaticus</t>
+  </si>
+  <si>
+    <t>Hypoxylon</t>
+  </si>
+  <si>
+    <t>Claviceps purpurea</t>
+  </si>
+  <si>
+    <t>Lachancea mirantina</t>
+  </si>
+  <si>
+    <t>Torrubiella hemipterigena</t>
+  </si>
+  <si>
+    <t>Laetiporus sulphureus</t>
+  </si>
+  <si>
+    <t>Aspergillus clavatus</t>
+  </si>
+  <si>
+    <t>Tremellales</t>
+  </si>
+  <si>
+    <t>Aspergillus nidulans</t>
+  </si>
+  <si>
+    <t>Aspergillus turcosus</t>
+  </si>
+  <si>
+    <t>[Candida] glabrata</t>
+  </si>
+  <si>
+    <t>Tetrapisispora blattae</t>
+  </si>
+  <si>
+    <t>Candida parapsilosis</t>
+  </si>
+  <si>
+    <t>Rhizoclosmatium globosum</t>
+  </si>
+  <si>
+    <t>Leucoagaricus sp. SymC.cos</t>
+  </si>
+  <si>
+    <t>Serpula lacrymans var. lacrymans</t>
+  </si>
+  <si>
+    <t>Calocera viscosa</t>
+  </si>
+  <si>
+    <t>Neolentinus lepideus</t>
+  </si>
+  <si>
+    <t>Paracoccidioides lutzii</t>
+  </si>
+  <si>
+    <t>Dothistroma septosporum</t>
+  </si>
+  <si>
+    <t>Bipolaris</t>
+  </si>
+  <si>
+    <t>Histoplasma capsulatum</t>
+  </si>
+  <si>
+    <t>Neocallimastigaceae</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps camponoti-rufipedis</t>
+  </si>
+  <si>
+    <t>Pestalotiopsis fici</t>
+  </si>
+  <si>
+    <t>Sporothrix</t>
+  </si>
+  <si>
+    <t>Blastomyces</t>
+  </si>
+  <si>
+    <t>Metarhizium robertsii</t>
+  </si>
+  <si>
+    <t>Trichophyton</t>
+  </si>
+  <si>
+    <t>Leptosphaeria maculans</t>
+  </si>
+  <si>
+    <t>Millerozyma farinosa</t>
+  </si>
+  <si>
+    <t>Hypocreomycetidae</t>
+  </si>
+  <si>
+    <t>Baudoinia panamericana</t>
+  </si>
+  <si>
+    <t>Schizosaccharomyces pombe</t>
+  </si>
+  <si>
+    <t>Mixia osmundae</t>
+  </si>
+  <si>
+    <t>Candida</t>
+  </si>
+  <si>
+    <t>Naumovozyma dairenensis</t>
+  </si>
+  <si>
+    <t>Ophiocordyceps unilateralis</t>
+  </si>
+  <si>
+    <t>Tuber aestivum</t>
+  </si>
+  <si>
+    <t>FEELVEAK</t>
+  </si>
+  <si>
+    <t>FGVYTMR</t>
+  </si>
+  <si>
+    <t>LEEELYHK</t>
+  </si>
+  <si>
+    <t>FPNFCPK</t>
+  </si>
+  <si>
+    <t>SMNTLER</t>
+  </si>
+  <si>
+    <t>WVEWVPR</t>
+  </si>
+  <si>
+    <t>VAQFRPR</t>
+  </si>
+  <si>
+    <t>YELQSPK</t>
+  </si>
+  <si>
+    <t>FLNFTSK</t>
+  </si>
+  <si>
+    <t>TPESAAVR</t>
+  </si>
+  <si>
+    <t>ETFAVLQK</t>
+  </si>
+  <si>
+    <t>MVVKPNK</t>
+  </si>
+  <si>
+    <t>TCMQQLLK</t>
+  </si>
+  <si>
+    <t>MALNRPTR</t>
+  </si>
+  <si>
+    <t>VGTFVFK</t>
+  </si>
+  <si>
+    <t>DGPVVWR</t>
+  </si>
+  <si>
+    <t>DLQALAPK</t>
+  </si>
+  <si>
+    <t>TQSHFEK</t>
+  </si>
+  <si>
+    <t>FELLGPPK</t>
+  </si>
+  <si>
+    <t>FLPYPAR</t>
+  </si>
+  <si>
+    <t>MADGDVPK</t>
+  </si>
+  <si>
+    <t>TNLTVAPGK</t>
+  </si>
+  <si>
+    <t>DLMTHEK</t>
+  </si>
+  <si>
+    <t>NFMLPNK</t>
+  </si>
+  <si>
+    <t>MCELHLHK</t>
+  </si>
+  <si>
+    <t>WYVSMR</t>
+  </si>
+  <si>
+    <t>RPLAGNK</t>
+  </si>
+  <si>
+    <t>HVVVFLR</t>
+  </si>
+  <si>
+    <t>EPLNNAK</t>
+  </si>
+  <si>
+    <t>TAGMTWK</t>
+  </si>
+  <si>
+    <t>MSPSMPR</t>
+  </si>
+  <si>
+    <t>NHCHVR</t>
+  </si>
+  <si>
+    <t>YWMTYK</t>
+  </si>
+  <si>
+    <t>MHCEPK</t>
+  </si>
+  <si>
+    <t>QTEGEAR</t>
+  </si>
+  <si>
+    <t>LMSEVHER</t>
+  </si>
+  <si>
+    <t>ACVYPK</t>
+  </si>
+  <si>
+    <t>MMAENTR</t>
+  </si>
+  <si>
+    <t>TMVYLDK</t>
+  </si>
+  <si>
+    <t>ESDMVPR</t>
+  </si>
+  <si>
+    <t>EPGLGYK</t>
+  </si>
+  <si>
+    <t>TGHLVYK</t>
+  </si>
+  <si>
+    <t>NPWHNK</t>
+  </si>
+  <si>
+    <t>FPLLTPLK</t>
+  </si>
+  <si>
+    <t>FMLQSNK</t>
+  </si>
+  <si>
+    <t>TLLYTENK</t>
+  </si>
+  <si>
+    <t>EEPNPMK</t>
+  </si>
+  <si>
+    <t>SYDDMTK</t>
+  </si>
+  <si>
+    <t>TLHQWMK</t>
+  </si>
+  <si>
+    <t>AAMTFPK</t>
+  </si>
+  <si>
+    <t>TLSTMPR</t>
+  </si>
+  <si>
+    <t>HLVVCNR</t>
+  </si>
+  <si>
+    <t>WNAMPPR</t>
+  </si>
+  <si>
+    <t>WWLLPQK</t>
+  </si>
+  <si>
+    <t>MQQHNFDK</t>
+  </si>
+  <si>
+    <t>EPAYVEK</t>
+  </si>
+  <si>
+    <t>WNVMVQR</t>
+  </si>
+  <si>
+    <t>LSSNPSAK</t>
+  </si>
+  <si>
+    <t>Penicillium digitatum</t>
+  </si>
+  <si>
+    <t>Ophiostoma piceae</t>
+  </si>
+  <si>
+    <t>Tilletia indica</t>
+  </si>
+  <si>
+    <t>Laccaria</t>
+  </si>
+  <si>
+    <t>Acremonium chrysogenum</t>
+  </si>
+  <si>
+    <t>Fistulina hepatica</t>
+  </si>
+  <si>
+    <t>Rhizophagus irregularis</t>
+  </si>
+  <si>
+    <t>Emergomyces pasteurianus</t>
+  </si>
+  <si>
+    <t>Cladophialophora immunda</t>
+  </si>
+  <si>
+    <t>Metschnikowia bicuspidata var. bicuspidata</t>
+  </si>
+  <si>
+    <t>Hypocrella siamensis</t>
+  </si>
+  <si>
+    <t>Neolecta irregularis</t>
+  </si>
+  <si>
+    <t>Agaricomycetidae</t>
+  </si>
+  <si>
+    <t>Pyrenophora tritici-repentis</t>
+  </si>
+  <si>
+    <t>Exophiala oligosperma</t>
+  </si>
+  <si>
+    <t>Basidiobolus meristosporus</t>
+  </si>
+  <si>
+    <t>Peniophora sp. CONT</t>
+  </si>
+  <si>
+    <t>Cordyceps fumosorosea</t>
+  </si>
+  <si>
+    <t>Auricularia subglabra</t>
+  </si>
+  <si>
+    <t>Phanerochaete carnosa</t>
+  </si>
+  <si>
+    <t>Conidiobolus coronatus</t>
+  </si>
+  <si>
+    <t>Piloderma croceum</t>
+  </si>
+  <si>
+    <t>Candida albicans</t>
+  </si>
+  <si>
+    <t>Pyronema omphalodes</t>
+  </si>
+  <si>
+    <t>Aureobasidium melanogenum</t>
+  </si>
+  <si>
+    <t>Cordyceps</t>
+  </si>
+  <si>
+    <t>Coniosporium apollinis</t>
+  </si>
+  <si>
+    <t>Cladophialophora bantiana</t>
+  </si>
+  <si>
+    <t>Moelleriella libera</t>
+  </si>
+  <si>
+    <t>Calocera</t>
+  </si>
+  <si>
+    <t>Talaromyces stipitatus</t>
+  </si>
+  <si>
+    <t>Moniliophthora perniciosa</t>
+  </si>
+  <si>
+    <t>Rosellinia necatrix</t>
+  </si>
+  <si>
+    <t>Beauveria bassiana</t>
+  </si>
+  <si>
+    <t>Acidomyces richmondensis</t>
+  </si>
+  <si>
+    <t>Colletotrichum gloeosporioides</t>
   </si>
 </sst>
 </file>
@@ -657,7 +1761,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,10 +1997,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39D6E-ADCE-C54E-86E3-C5932C98575B}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,16 +2012,17 @@
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="12" width="16.6640625" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="16.1640625" customWidth="1"/>
+    <col min="8" max="8" width="16" customWidth="1"/>
+    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="10" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="17" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+    <col min="15" max="15" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -940,220 +2045,2636 @@
         <v>32</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F2" t="s">
+        <v>360</v>
+      </c>
+      <c r="G2" t="s">
+        <v>99</v>
+      </c>
       <c r="H2" t="s">
+        <v>125</v>
+      </c>
+      <c r="I2" t="s">
         <v>62</v>
-      </c>
-      <c r="I2" t="s">
-        <v>63</v>
       </c>
       <c r="J2" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="K2" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" t="s">
+        <v>87</v>
+      </c>
+      <c r="M2" t="s">
+        <v>86</v>
+      </c>
+      <c r="N2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" t="s">
+        <v>244</v>
+      </c>
+      <c r="F3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G3" t="s">
+        <v>100</v>
+      </c>
       <c r="H3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" t="s">
         <v>63</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>80</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="L3" t="s">
+        <v>86</v>
+      </c>
+      <c r="M3" t="s">
+        <v>87</v>
+      </c>
+      <c r="N3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F4" t="s">
+        <v>362</v>
+      </c>
+      <c r="G4" t="s">
+        <v>101</v>
+      </c>
       <c r="H4" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" t="s">
         <v>64</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>81</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="L4" t="s">
+        <v>96</v>
+      </c>
+      <c r="M4" t="s">
+        <v>88</v>
+      </c>
+      <c r="N4" t="s">
+        <v>86</v>
+      </c>
+      <c r="O4" t="s">
+        <v>64</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E5" t="s">
+        <v>246</v>
+      </c>
+      <c r="F5" t="s">
+        <v>363</v>
+      </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
       <c r="H5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I5" t="s">
         <v>65</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>82</v>
       </c>
-      <c r="O5" s="2" t="s">
+      <c r="M5" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" t="s">
+        <v>189</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" t="s">
+        <v>247</v>
+      </c>
+      <c r="F6" t="s">
+        <v>364</v>
+      </c>
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
       <c r="H6" t="s">
+        <v>129</v>
+      </c>
+      <c r="I6" t="s">
         <v>66</v>
       </c>
-      <c r="O6" s="2" t="s">
+      <c r="O6" t="s">
+        <v>66</v>
+      </c>
+      <c r="P6" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+      <c r="D7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" t="s">
+        <v>248</v>
+      </c>
+      <c r="F7" t="s">
+        <v>365</v>
+      </c>
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
       <c r="H7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" t="s">
         <v>67</v>
       </c>
-      <c r="O7" s="2" t="s">
+      <c r="O7" t="s">
+        <v>67</v>
+      </c>
+      <c r="P7" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" t="s">
+        <v>191</v>
+      </c>
+      <c r="D8" t="s">
+        <v>213</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F8" t="s">
+        <v>366</v>
+      </c>
+      <c r="G8" t="s">
+        <v>105</v>
+      </c>
       <c r="H8" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" t="s">
         <v>68</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="O8" t="s">
+        <v>68</v>
+      </c>
+      <c r="P8" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E9" t="s">
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
+        <v>367</v>
+      </c>
+      <c r="G9" t="s">
+        <v>106</v>
+      </c>
       <c r="H9" t="s">
+        <v>131</v>
+      </c>
+      <c r="I9" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="2" t="s">
+      <c r="O9" t="s">
+        <v>69</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B10" t="s">
+        <v>157</v>
+      </c>
+      <c r="C10" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" t="s">
+        <v>215</v>
+      </c>
+      <c r="E10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F10" t="s">
+        <v>368</v>
+      </c>
+      <c r="G10" t="s">
+        <v>107</v>
+      </c>
       <c r="H10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I10" t="s">
         <v>70</v>
       </c>
-      <c r="O10" s="2" t="s">
+      <c r="O10" t="s">
+        <v>70</v>
+      </c>
+      <c r="P10" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" t="s">
+        <v>194</v>
+      </c>
+      <c r="D11" t="s">
+        <v>216</v>
+      </c>
+      <c r="E11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F11" t="s">
+        <v>369</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
       <c r="H11" t="s">
+        <v>133</v>
+      </c>
+      <c r="I11" t="s">
         <v>71</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="O11" t="s">
+        <v>71</v>
+      </c>
+      <c r="P11" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>109</v>
+      </c>
+      <c r="B12" t="s">
+        <v>159</v>
+      </c>
+      <c r="C12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D12" t="s">
+        <v>217</v>
+      </c>
+      <c r="E12" t="s">
+        <v>253</v>
+      </c>
+      <c r="F12" t="s">
+        <v>370</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
       <c r="H12" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" t="s">
         <v>72</v>
       </c>
-      <c r="O12" s="2" t="s">
+      <c r="O12" t="s">
+        <v>72</v>
+      </c>
+      <c r="P12" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E13" t="s">
+        <v>254</v>
+      </c>
+      <c r="F13" t="s">
+        <v>371</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
       <c r="H13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I13" t="s">
         <v>73</v>
       </c>
-      <c r="O13" s="2" t="s">
+      <c r="O13" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>111</v>
+      </c>
+      <c r="B14" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" t="s">
+        <v>197</v>
+      </c>
+      <c r="D14" t="s">
+        <v>219</v>
+      </c>
+      <c r="E14" t="s">
+        <v>255</v>
+      </c>
+      <c r="F14" t="s">
+        <v>372</v>
+      </c>
+      <c r="G14" t="s">
+        <v>111</v>
+      </c>
       <c r="H14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I14" t="s">
         <v>74</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="O14" t="s">
+        <v>74</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" t="s">
+        <v>256</v>
+      </c>
+      <c r="F15" t="s">
+        <v>373</v>
+      </c>
+      <c r="G15" t="s">
+        <v>112</v>
+      </c>
       <c r="H15" t="s">
+        <v>137</v>
+      </c>
+      <c r="I15" t="s">
         <v>75</v>
       </c>
-      <c r="O15" s="2" t="s">
+      <c r="O15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P15" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" t="s">
+        <v>221</v>
+      </c>
+      <c r="E16" t="s">
+        <v>257</v>
+      </c>
+      <c r="F16" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
       <c r="H16" t="s">
+        <v>138</v>
+      </c>
+      <c r="I16" t="s">
         <v>76</v>
       </c>
-      <c r="O16" s="2" t="s">
+      <c r="O16" t="s">
+        <v>76</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" t="s">
+        <v>164</v>
+      </c>
+      <c r="D17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F17" t="s">
+        <v>374</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
       <c r="H17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" t="s">
         <v>77</v>
       </c>
-      <c r="O17" s="2" t="s">
+      <c r="O17" t="s">
+        <v>77</v>
+      </c>
+      <c r="P17" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" t="s">
+        <v>223</v>
+      </c>
+      <c r="E18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" t="s">
+        <v>375</v>
+      </c>
+      <c r="G18" t="s">
+        <v>115</v>
+      </c>
       <c r="H18" t="s">
+        <v>140</v>
+      </c>
+      <c r="I18" t="s">
         <v>78</v>
       </c>
-      <c r="O18" s="2" t="s">
+      <c r="O18" t="s">
+        <v>78</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19" t="s">
+        <v>166</v>
+      </c>
+      <c r="D19" t="s">
+        <v>224</v>
+      </c>
+      <c r="E19" t="s">
+        <v>260</v>
+      </c>
+      <c r="F19" t="s">
+        <v>376</v>
+      </c>
+      <c r="G19" t="s">
+        <v>116</v>
+      </c>
       <c r="H19" t="s">
+        <v>141</v>
+      </c>
+      <c r="I19" t="s">
         <v>79</v>
       </c>
-      <c r="O19" s="2" t="s">
+      <c r="O19" t="s">
+        <v>79</v>
+      </c>
+      <c r="P19" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="D20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E20" t="s">
+        <v>261</v>
+      </c>
+      <c r="F20" t="s">
+        <v>377</v>
+      </c>
+      <c r="G20" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" t="s">
+        <v>142</v>
+      </c>
       <c r="O20" t="s">
+        <v>63</v>
+      </c>
+      <c r="P20" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>168</v>
+      </c>
+      <c r="D21" t="s">
+        <v>226</v>
+      </c>
+      <c r="E21" t="s">
+        <v>262</v>
+      </c>
+      <c r="F21" t="s">
+        <v>378</v>
+      </c>
+      <c r="G21" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" t="s">
+        <v>143</v>
+      </c>
       <c r="O21" t="s">
+        <v>80</v>
+      </c>
+      <c r="P21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>119</v>
+      </c>
+      <c r="B22" t="s">
+        <v>169</v>
+      </c>
+      <c r="E22" t="s">
+        <v>263</v>
+      </c>
+      <c r="F22" t="s">
+        <v>379</v>
+      </c>
+      <c r="G22" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" t="s">
+        <v>144</v>
+      </c>
       <c r="O22" t="s">
+        <v>81</v>
+      </c>
+      <c r="P22" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>120</v>
+      </c>
+      <c r="B23" t="s">
+        <v>170</v>
+      </c>
+      <c r="E23" t="s">
+        <v>264</v>
+      </c>
+      <c r="F23" t="s">
+        <v>380</v>
+      </c>
+      <c r="G23" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" t="s">
+        <v>145</v>
+      </c>
       <c r="O23" t="s">
+        <v>82</v>
+      </c>
+      <c r="P23" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="24" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" t="s">
+        <v>265</v>
+      </c>
+      <c r="F24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24" t="s">
+        <v>146</v>
+      </c>
       <c r="O24" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="8:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" t="s">
+        <v>266</v>
+      </c>
+      <c r="F25" t="s">
+        <v>382</v>
+      </c>
+      <c r="G25" t="s">
+        <v>122</v>
+      </c>
+      <c r="H25" t="s">
+        <v>147</v>
+      </c>
       <c r="O25" t="s">
+        <v>66</v>
+      </c>
+      <c r="P25" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>123</v>
+      </c>
+      <c r="E26" t="s">
+        <v>267</v>
+      </c>
+      <c r="F26" t="s">
+        <v>383</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26" t="s">
+        <v>148</v>
+      </c>
+      <c r="O26" t="s">
+        <v>87</v>
+      </c>
+      <c r="P26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>124</v>
+      </c>
+      <c r="E27" t="s">
+        <v>268</v>
+      </c>
+      <c r="F27" t="s">
+        <v>163</v>
+      </c>
+      <c r="G27" t="s">
+        <v>124</v>
+      </c>
+      <c r="H27" t="s">
+        <v>149</v>
+      </c>
+      <c r="O27" t="s">
+        <v>86</v>
+      </c>
+      <c r="P27" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>269</v>
+      </c>
+      <c r="F28" t="s">
+        <v>384</v>
+      </c>
+      <c r="G28" t="s">
+        <v>150</v>
+      </c>
+      <c r="H28" t="s">
+        <v>171</v>
+      </c>
+      <c r="O28" t="s">
+        <v>96</v>
+      </c>
+      <c r="P28" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>270</v>
+      </c>
+      <c r="F29" t="s">
+        <v>385</v>
+      </c>
+      <c r="G29" t="s">
+        <v>100</v>
+      </c>
+      <c r="H29" t="s">
+        <v>126</v>
+      </c>
+      <c r="O29" t="s">
+        <v>86</v>
+      </c>
+      <c r="P29" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>271</v>
+      </c>
+      <c r="F30" t="s">
+        <v>386</v>
+      </c>
+      <c r="G30" t="s">
+        <v>151</v>
+      </c>
+      <c r="H30" t="s">
+        <v>53</v>
+      </c>
+      <c r="O30" t="s">
+        <v>87</v>
+      </c>
+      <c r="P30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>272</v>
+      </c>
+      <c r="F31" t="s">
+        <v>387</v>
+      </c>
+      <c r="G31" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" t="s">
+        <v>172</v>
+      </c>
+      <c r="O31" t="s">
+        <v>88</v>
+      </c>
+      <c r="P31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="E32" t="s">
+        <v>273</v>
+      </c>
+      <c r="F32" t="s">
+        <v>388</v>
+      </c>
+      <c r="G32" t="s">
+        <v>153</v>
+      </c>
+      <c r="H32" t="s">
+        <v>53</v>
+      </c>
+      <c r="O32" t="s">
+        <v>89</v>
+      </c>
+      <c r="P32" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="33" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E33" t="s">
+        <v>274</v>
+      </c>
+      <c r="F33" t="s">
+        <v>389</v>
+      </c>
+      <c r="G33" t="s">
+        <v>154</v>
+      </c>
+      <c r="H33" t="s">
+        <v>173</v>
+      </c>
+      <c r="O33" t="s">
+        <v>64</v>
+      </c>
+      <c r="P33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E34" t="s">
+        <v>275</v>
+      </c>
+      <c r="F34" t="s">
+        <v>113</v>
+      </c>
+      <c r="G34" t="s">
+        <v>155</v>
+      </c>
+      <c r="H34" t="s">
+        <v>174</v>
+      </c>
+      <c r="O34" t="s">
+        <v>94</v>
+      </c>
+      <c r="P34" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E35" t="s">
+        <v>276</v>
+      </c>
+      <c r="F35" t="s">
+        <v>390</v>
+      </c>
+      <c r="G35" t="s">
+        <v>156</v>
+      </c>
+      <c r="H35" t="s">
+        <v>57</v>
+      </c>
+      <c r="O35" t="s">
+        <v>86</v>
+      </c>
+      <c r="P35" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>277</v>
+      </c>
+      <c r="F36" t="s">
+        <v>391</v>
+      </c>
+      <c r="G36" t="s">
+        <v>157</v>
+      </c>
+      <c r="H36" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="37" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E37" t="s">
+        <v>278</v>
+      </c>
+      <c r="F37" t="s">
+        <v>392</v>
+      </c>
+      <c r="G37" t="s">
+        <v>158</v>
+      </c>
+      <c r="H37" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="38" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E38" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" t="s">
+        <v>393</v>
+      </c>
+      <c r="G38" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E39" t="s">
+        <v>280</v>
+      </c>
+      <c r="F39" t="s">
+        <v>394</v>
+      </c>
+      <c r="G39" t="s">
+        <v>160</v>
+      </c>
+      <c r="H39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E40" t="s">
+        <v>281</v>
+      </c>
+      <c r="F40" t="s">
+        <v>395</v>
+      </c>
+      <c r="G40" t="s">
+        <v>161</v>
+      </c>
+      <c r="H40" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="41" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>282</v>
+      </c>
+      <c r="F41" t="s">
+        <v>396</v>
+      </c>
+      <c r="G41" t="s">
+        <v>162</v>
+      </c>
+      <c r="H41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E42" t="s">
+        <v>283</v>
+      </c>
+      <c r="F42" t="s">
+        <v>397</v>
+      </c>
+      <c r="G42" t="s">
+        <v>163</v>
+      </c>
+      <c r="H42" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="43" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E43" t="s">
+        <v>284</v>
+      </c>
+      <c r="F43" t="s">
+        <v>398</v>
+      </c>
+      <c r="G43" t="s">
+        <v>164</v>
+      </c>
+      <c r="H43" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E44" t="s">
+        <v>285</v>
+      </c>
+      <c r="F44" t="s">
+        <v>399</v>
+      </c>
+      <c r="G44" t="s">
+        <v>165</v>
+      </c>
+      <c r="H44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E45" t="s">
+        <v>286</v>
+      </c>
+      <c r="F45" t="s">
+        <v>400</v>
+      </c>
+      <c r="G45" t="s">
+        <v>166</v>
+      </c>
+      <c r="H45" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="46" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>287</v>
+      </c>
+      <c r="F46" t="s">
+        <v>401</v>
+      </c>
+      <c r="G46" t="s">
+        <v>167</v>
+      </c>
+      <c r="H46" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E47" t="s">
+        <v>288</v>
+      </c>
+      <c r="F47" t="s">
+        <v>402</v>
+      </c>
+      <c r="G47" t="s">
+        <v>168</v>
+      </c>
+      <c r="H47" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="5:16" x14ac:dyDescent="0.2">
+      <c r="E48" t="s">
+        <v>289</v>
+      </c>
+      <c r="F48" t="s">
+        <v>403</v>
+      </c>
+      <c r="G48" t="s">
+        <v>169</v>
+      </c>
+      <c r="H48" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E49" t="s">
+        <v>290</v>
+      </c>
+      <c r="F49" t="s">
+        <v>404</v>
+      </c>
+      <c r="G49" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="50" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E50" t="s">
+        <v>291</v>
+      </c>
+      <c r="F50" t="s">
+        <v>405</v>
+      </c>
+      <c r="G50" t="s">
+        <v>186</v>
+      </c>
+      <c r="H50" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E51" t="s">
+        <v>292</v>
+      </c>
+      <c r="F51" t="s">
+        <v>406</v>
+      </c>
+      <c r="G51" t="s">
+        <v>187</v>
+      </c>
+      <c r="H51" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E52" t="s">
+        <v>293</v>
+      </c>
+      <c r="F52" t="s">
+        <v>407</v>
+      </c>
+      <c r="G52" t="s">
+        <v>188</v>
+      </c>
+      <c r="H52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E53" t="s">
+        <v>294</v>
+      </c>
+      <c r="F53" t="s">
+        <v>408</v>
+      </c>
+      <c r="G53" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E54" t="s">
+        <v>295</v>
+      </c>
+      <c r="F54" t="s">
+        <v>409</v>
+      </c>
+      <c r="G54" t="s">
+        <v>189</v>
+      </c>
+      <c r="H54" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="55" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E55" t="s">
+        <v>296</v>
+      </c>
+      <c r="F55" t="s">
+        <v>410</v>
+      </c>
+      <c r="G55" t="s">
+        <v>190</v>
+      </c>
+      <c r="H55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E56" t="s">
+        <v>297</v>
+      </c>
+      <c r="F56" t="s">
+        <v>411</v>
+      </c>
+      <c r="G56" t="s">
+        <v>191</v>
+      </c>
+      <c r="H56" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="57" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E57" t="s">
+        <v>298</v>
+      </c>
+      <c r="F57" t="s">
+        <v>412</v>
+      </c>
+      <c r="G57" t="s">
+        <v>192</v>
+      </c>
+      <c r="H57" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="58" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E58" t="s">
+        <v>299</v>
+      </c>
+      <c r="F58" t="s">
+        <v>413</v>
+      </c>
+      <c r="G58" t="s">
+        <v>193</v>
+      </c>
+      <c r="H58" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="59" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>300</v>
+      </c>
+      <c r="F59" t="s">
+        <v>414</v>
+      </c>
+      <c r="G59" t="s">
+        <v>194</v>
+      </c>
+      <c r="H59" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="60" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E60" t="s">
+        <v>301</v>
+      </c>
+      <c r="F60" t="s">
+        <v>415</v>
+      </c>
+      <c r="G60" t="s">
+        <v>195</v>
+      </c>
+      <c r="H60" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="61" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E61" t="s">
+        <v>302</v>
+      </c>
+      <c r="F61" t="s">
+        <v>416</v>
+      </c>
+      <c r="G61" t="s">
+        <v>196</v>
+      </c>
+      <c r="H61" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="62" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E62" t="s">
+        <v>303</v>
+      </c>
+      <c r="F62" t="s">
+        <v>417</v>
+      </c>
+      <c r="G62" t="s">
+        <v>197</v>
+      </c>
+      <c r="H62" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="63" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>304</v>
+      </c>
+      <c r="G63" t="s">
+        <v>208</v>
+      </c>
+      <c r="H63" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="64" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E64" t="s">
+        <v>305</v>
+      </c>
+      <c r="G64" t="s">
+        <v>100</v>
+      </c>
+      <c r="H64" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E65" t="s">
+        <v>306</v>
+      </c>
+      <c r="G65" t="s">
+        <v>209</v>
+      </c>
+      <c r="H65" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="66" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E66" t="s">
+        <v>307</v>
+      </c>
+      <c r="G66" t="s">
+        <v>210</v>
+      </c>
+      <c r="H66" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="67" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E67" t="s">
+        <v>308</v>
+      </c>
+      <c r="G67" t="s">
+        <v>211</v>
+      </c>
+      <c r="H67" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="68" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E68" t="s">
+        <v>309</v>
+      </c>
+      <c r="G68" t="s">
+        <v>212</v>
+      </c>
+      <c r="H68" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="69" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G69" t="s">
+        <v>213</v>
+      </c>
+      <c r="H69" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G70" t="s">
+        <v>214</v>
+      </c>
+      <c r="H70" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G71" t="s">
+        <v>215</v>
+      </c>
+      <c r="H71" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="72" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G72" t="s">
+        <v>216</v>
+      </c>
+      <c r="H72" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="73" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G73" t="s">
+        <v>217</v>
+      </c>
+      <c r="H73" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="74" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G74" t="s">
+        <v>218</v>
+      </c>
+      <c r="H74" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="75" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G75" t="s">
+        <v>219</v>
+      </c>
+      <c r="H75" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="76" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G76" t="s">
+        <v>220</v>
+      </c>
+      <c r="H76" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="77" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G77" t="s">
+        <v>221</v>
+      </c>
+      <c r="H77" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G78" t="s">
+        <v>222</v>
+      </c>
+      <c r="H78" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="79" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G79" t="s">
+        <v>223</v>
+      </c>
+      <c r="H79" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="80" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="G80" t="s">
+        <v>224</v>
+      </c>
+      <c r="H80" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="81" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G81" t="s">
+        <v>225</v>
+      </c>
+      <c r="H81" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="82" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G82" t="s">
+        <v>226</v>
+      </c>
+      <c r="H82" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="83" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G83" t="s">
+        <v>243</v>
+      </c>
+      <c r="H83" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="84" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G84" t="s">
+        <v>244</v>
+      </c>
+      <c r="H84" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="85" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G85" t="s">
+        <v>245</v>
+      </c>
+      <c r="H85" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="86" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G86" t="s">
+        <v>246</v>
+      </c>
+      <c r="H86" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="87" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G87" t="s">
+        <v>247</v>
+      </c>
+      <c r="H87" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="88" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G88" t="s">
+        <v>248</v>
+      </c>
+      <c r="H88" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="89" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G89" t="s">
+        <v>249</v>
+      </c>
+      <c r="H89" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="90" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G90" t="s">
+        <v>250</v>
+      </c>
+      <c r="H90" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="91" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G91" t="s">
+        <v>251</v>
+      </c>
+      <c r="H91" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="92" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G92" t="s">
+        <v>252</v>
+      </c>
+      <c r="H92" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="93" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G93" t="s">
+        <v>253</v>
+      </c>
+      <c r="H93" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="94" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G94" t="s">
+        <v>254</v>
+      </c>
+      <c r="H94" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="95" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G95" t="s">
+        <v>255</v>
+      </c>
+      <c r="H95" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="96" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G96" t="s">
+        <v>256</v>
+      </c>
+      <c r="H96" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G97" t="s">
+        <v>257</v>
+      </c>
+      <c r="H97" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="98" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G98" t="s">
+        <v>258</v>
+      </c>
+      <c r="H98" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="99" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G99" t="s">
+        <v>259</v>
+      </c>
+      <c r="H99" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="100" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G100" t="s">
+        <v>260</v>
+      </c>
+      <c r="H100" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="101" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G101" t="s">
+        <v>261</v>
+      </c>
+      <c r="H101" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="102" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G102" t="s">
+        <v>262</v>
+      </c>
+      <c r="H102" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="103" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G103" t="s">
+        <v>263</v>
+      </c>
+      <c r="H103" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="104" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G104" t="s">
+        <v>264</v>
+      </c>
+      <c r="H104" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="105" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G105" t="s">
+        <v>265</v>
+      </c>
+      <c r="H105" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="106" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G106" t="s">
+        <v>266</v>
+      </c>
+      <c r="H106" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="107" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G107" t="s">
+        <v>267</v>
+      </c>
+      <c r="H107" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="108" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G108" t="s">
+        <v>268</v>
+      </c>
+      <c r="H108" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="109" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G109" t="s">
+        <v>269</v>
+      </c>
+      <c r="H109" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="110" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G110" t="s">
+        <v>270</v>
+      </c>
+      <c r="H110" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="111" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G111" t="s">
+        <v>271</v>
+      </c>
+      <c r="H111" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="112" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G112" t="s">
+        <v>272</v>
+      </c>
+      <c r="H112" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="113" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G113" t="s">
+        <v>273</v>
+      </c>
+      <c r="H113" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="114" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G114" t="s">
+        <v>274</v>
+      </c>
+      <c r="H114" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G115" t="s">
+        <v>275</v>
+      </c>
+      <c r="H115" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="116" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G116" t="s">
+        <v>276</v>
+      </c>
+      <c r="H116" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="117" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G117" t="s">
+        <v>277</v>
+      </c>
+      <c r="H117" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="118" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G118" t="s">
+        <v>278</v>
+      </c>
+      <c r="H118" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="119" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G119" t="s">
+        <v>279</v>
+      </c>
+      <c r="H119" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="120" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G120" t="s">
+        <v>280</v>
+      </c>
+      <c r="H120" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="121" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G121" t="s">
+        <v>281</v>
+      </c>
+      <c r="H121" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="122" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G122" t="s">
+        <v>282</v>
+      </c>
+      <c r="H122" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="123" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G123" t="s">
+        <v>283</v>
+      </c>
+      <c r="H123" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="124" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G124" t="s">
+        <v>284</v>
+      </c>
+      <c r="H124" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="125" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G125" t="s">
+        <v>285</v>
+      </c>
+      <c r="H125" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="126" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G126" t="s">
+        <v>286</v>
+      </c>
+      <c r="H126" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="127" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G127" t="s">
+        <v>287</v>
+      </c>
+      <c r="H127" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="128" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G128" t="s">
+        <v>288</v>
+      </c>
+      <c r="H128" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="129" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G129" t="s">
+        <v>289</v>
+      </c>
+      <c r="H129" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="130" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G130" t="s">
+        <v>290</v>
+      </c>
+      <c r="H130" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="131" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G131" t="s">
+        <v>291</v>
+      </c>
+      <c r="H131" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="132" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G132" t="s">
+        <v>292</v>
+      </c>
+      <c r="H132" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="133" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G133" t="s">
+        <v>293</v>
+      </c>
+      <c r="H133" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="134" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G134" t="s">
+        <v>294</v>
+      </c>
+      <c r="H134" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="135" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G135" t="s">
+        <v>295</v>
+      </c>
+      <c r="H135" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="136" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G136" t="s">
+        <v>296</v>
+      </c>
+      <c r="H136" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="137" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G137" t="s">
+        <v>297</v>
+      </c>
+      <c r="H137" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="138" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G138" t="s">
+        <v>298</v>
+      </c>
+      <c r="H138" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="139" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G139" t="s">
+        <v>299</v>
+      </c>
+      <c r="H139" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="140" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G140" t="s">
+        <v>300</v>
+      </c>
+      <c r="H140" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="141" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G141" t="s">
+        <v>301</v>
+      </c>
+      <c r="H141" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="142" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G142" t="s">
+        <v>302</v>
+      </c>
+      <c r="H142" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="143" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G143" t="s">
+        <v>303</v>
+      </c>
+      <c r="H143" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="144" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G144" t="s">
+        <v>304</v>
+      </c>
+      <c r="H144" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="145" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G145" t="s">
+        <v>305</v>
+      </c>
+      <c r="H145" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="146" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G146" t="s">
+        <v>306</v>
+      </c>
+      <c r="H146" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="147" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G147" t="s">
+        <v>307</v>
+      </c>
+      <c r="H147" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="148" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G148" t="s">
+        <v>308</v>
+      </c>
+      <c r="H148" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="149" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G149" t="s">
+        <v>309</v>
+      </c>
+      <c r="H149" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="150" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G150" t="s">
+        <v>360</v>
+      </c>
+      <c r="H150" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="151" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G151" t="s">
+        <v>361</v>
+      </c>
+      <c r="H151" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="152" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G152" t="s">
+        <v>362</v>
+      </c>
+      <c r="H152" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="153" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G153" t="s">
+        <v>363</v>
+      </c>
+      <c r="H153" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="154" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G154" t="s">
+        <v>364</v>
+      </c>
+      <c r="H154" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="155" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G155" t="s">
+        <v>365</v>
+      </c>
+      <c r="H155" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="156" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G156" t="s">
+        <v>366</v>
+      </c>
+      <c r="H156" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="157" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G157" t="s">
+        <v>367</v>
+      </c>
+      <c r="H157" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="158" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G158" t="s">
+        <v>368</v>
+      </c>
+      <c r="H158" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="159" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G159" t="s">
+        <v>369</v>
+      </c>
+      <c r="H159" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="160" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G160" t="s">
+        <v>370</v>
+      </c>
+      <c r="H160" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="161" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G161" t="s">
+        <v>371</v>
+      </c>
+      <c r="H161" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="162" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G162" t="s">
+        <v>372</v>
+      </c>
+      <c r="H162" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="163" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G163" t="s">
+        <v>373</v>
+      </c>
+      <c r="H163" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="164" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G164" t="s">
+        <v>100</v>
+      </c>
+      <c r="H164" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="165" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G165" t="s">
+        <v>374</v>
+      </c>
+      <c r="H165" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="166" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G166" t="s">
+        <v>375</v>
+      </c>
+      <c r="H166" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="167" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G167" t="s">
+        <v>376</v>
+      </c>
+      <c r="H167" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="168" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G168" t="s">
+        <v>377</v>
+      </c>
+      <c r="H168" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="169" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G169" t="s">
+        <v>378</v>
+      </c>
+      <c r="H169" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="170" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G170" t="s">
+        <v>379</v>
+      </c>
+      <c r="H170" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="171" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G171" t="s">
+        <v>380</v>
+      </c>
+      <c r="H171" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="172" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G172" t="s">
+        <v>381</v>
+      </c>
+      <c r="H172" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="173" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G173" t="s">
+        <v>382</v>
+      </c>
+      <c r="H173" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="174" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G174" t="s">
+        <v>383</v>
+      </c>
+      <c r="H174" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="175" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G175" t="s">
+        <v>163</v>
+      </c>
+      <c r="H175" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="176" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G176" t="s">
+        <v>384</v>
+      </c>
+      <c r="H176" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="177" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G177" t="s">
+        <v>385</v>
+      </c>
+      <c r="H177" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="178" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G178" t="s">
+        <v>386</v>
+      </c>
+      <c r="H178" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="179" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G179" t="s">
+        <v>387</v>
+      </c>
+      <c r="H179" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="180" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G180" t="s">
+        <v>388</v>
+      </c>
+      <c r="H180" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="181" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G181" t="s">
+        <v>389</v>
+      </c>
+      <c r="H181" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="182" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G182" t="s">
+        <v>113</v>
+      </c>
+      <c r="H182" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="183" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G183" t="s">
+        <v>390</v>
+      </c>
+      <c r="H183" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="184" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G184" t="s">
+        <v>391</v>
+      </c>
+      <c r="H184" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="185" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G185" t="s">
+        <v>392</v>
+      </c>
+      <c r="H185" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="186" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G186" t="s">
+        <v>393</v>
+      </c>
+      <c r="H186" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="187" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G187" t="s">
+        <v>394</v>
+      </c>
+      <c r="H187" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="188" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G188" t="s">
+        <v>395</v>
+      </c>
+      <c r="H188" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="189" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G189" t="s">
+        <v>396</v>
+      </c>
+      <c r="H189" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="190" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G190" t="s">
+        <v>397</v>
+      </c>
+      <c r="H190" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="191" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G191" t="s">
+        <v>398</v>
+      </c>
+      <c r="H191" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="192" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G192" t="s">
+        <v>399</v>
+      </c>
+      <c r="H192" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="193" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G193" t="s">
+        <v>400</v>
+      </c>
+      <c r="H193" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="194" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G194" t="s">
+        <v>401</v>
+      </c>
+      <c r="H194" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="195" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G195" t="s">
+        <v>402</v>
+      </c>
+      <c r="H195" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="196" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G196" t="s">
+        <v>403</v>
+      </c>
+      <c r="H196" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="197" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G197" t="s">
+        <v>404</v>
+      </c>
+      <c r="H197" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="198" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G198" t="s">
+        <v>405</v>
+      </c>
+      <c r="H198" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="199" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G199" t="s">
+        <v>406</v>
+      </c>
+      <c r="H199" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="200" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G200" t="s">
+        <v>407</v>
+      </c>
+      <c r="H200" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="201" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G201" t="s">
+        <v>408</v>
+      </c>
+      <c r="H201" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="202" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G202" t="s">
+        <v>409</v>
+      </c>
+      <c r="H202" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="203" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G203" t="s">
+        <v>410</v>
+      </c>
+      <c r="H203" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="204" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G204" t="s">
+        <v>411</v>
+      </c>
+      <c r="H204" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="205" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G205" t="s">
+        <v>412</v>
+      </c>
+      <c r="H205" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="206" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G206" t="s">
+        <v>413</v>
+      </c>
+      <c r="H206" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="207" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G207" t="s">
+        <v>414</v>
+      </c>
+      <c r="H207" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="208" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G208" t="s">
+        <v>415</v>
+      </c>
+      <c r="H208" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="209" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G209" t="s">
+        <v>416</v>
+      </c>
+      <c r="H209" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="210" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G210" t="s">
+        <v>417</v>
+      </c>
+      <c r="H210" t="s">
+        <v>176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cyano fungi workup redid
</commit_message>
<xml_diff>
--- a/analyses/pronovo-2019/cyano-fungi-workup.xlsx
+++ b/analyses/pronovo-2019/cyano-fungi-workup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/pronovo-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B228A9D-0699-BA42-9B4B-7CDAE9385034}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B72F28-0FF6-EF44-8623-451AA6135642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
   </bookViews>
   <sheets>
     <sheet name="cyano dno + db peps tryptic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="558">
   <si>
     <t>LASGLDAVTK</t>
   </si>
@@ -1396,6 +1396,318 @@
   </si>
   <si>
     <t>Colletotrichum gloeosporioides</t>
+  </si>
+  <si>
+    <t>ALTTGVDYAQGLVALGGDDK</t>
+  </si>
+  <si>
+    <t>AYTALLDLKPGDEFELK</t>
+  </si>
+  <si>
+    <t>LAENAGANGAVVAENVK</t>
+  </si>
+  <si>
+    <t>LDLNNASVR</t>
+  </si>
+  <si>
+    <t>LGGDEYVLLSEK</t>
+  </si>
+  <si>
+    <t>LVVGGPYSSVSDASSGLDGSQK</t>
+  </si>
+  <si>
+    <t>QAPEVGVGDNVLYSK</t>
+  </si>
+  <si>
+    <t>TGGDPLELFETAVK</t>
+  </si>
+  <si>
+    <t>TNQNVGLDPETLALATPAR</t>
+  </si>
+  <si>
+    <t>VFPGGDTEFLHPK</t>
+  </si>
+  <si>
+    <t>VLQQEGFLSELSEEGEGVR</t>
+  </si>
+  <si>
+    <t>YLGSTGGLLNSAETEEK</t>
+  </si>
+  <si>
+    <t>YNSGEGGCFYSVDTLEAPWNSGR</t>
+  </si>
+  <si>
+    <t>AAVEQLFDVR</t>
+  </si>
+  <si>
+    <t>ALATSDLGLTPNNDGK</t>
+  </si>
+  <si>
+    <t>ALVNNLPLYR</t>
+  </si>
+  <si>
+    <t>ASAADTPQALAR</t>
+  </si>
+  <si>
+    <t>DLNYYSALYEK</t>
+  </si>
+  <si>
+    <t>LGADEYVLLSEK</t>
+  </si>
+  <si>
+    <t>LLSQAFGLLNER</t>
+  </si>
+  <si>
+    <t>LVADEESTSPEVSTVEEEELSALMGEK</t>
+  </si>
+  <si>
+    <t>VPTPNVSAVDLVFESGR</t>
+  </si>
+  <si>
+    <t>VQDYAELDGAPEER</t>
+  </si>
+  <si>
+    <t>YVSYAVLAGDASVLQDR</t>
+  </si>
+  <si>
+    <t>AYTALLDLK</t>
+  </si>
+  <si>
+    <t>DAFLYYPLQYEGQECSK</t>
+  </si>
+  <si>
+    <t>DHVPADFEK</t>
+  </si>
+  <si>
+    <t>LQNDVQPWQVR</t>
+  </si>
+  <si>
+    <t>SVSVSNVGTVLQLGDGLAR</t>
+  </si>
+  <si>
+    <t>TSDTDGYAAVQLGFGDTR</t>
+  </si>
+  <si>
+    <t>VVDADGTQLGVLNR</t>
+  </si>
+  <si>
+    <t>AAGFALTEAEVK</t>
+  </si>
+  <si>
+    <t>AVASGSVSAEK</t>
+  </si>
+  <si>
+    <t>FDNADLSNANFSGAELLK</t>
+  </si>
+  <si>
+    <t>FEQPGFFSK</t>
+  </si>
+  <si>
+    <t>GSLPQNLGSTGGLLNSAETEEK</t>
+  </si>
+  <si>
+    <t>LDHSQLLTDPAEAADFVAK</t>
+  </si>
+  <si>
+    <t>LLDQDGVPVVFGGWTSASR</t>
+  </si>
+  <si>
+    <t>LNVEYYGTETPLK</t>
+  </si>
+  <si>
+    <t>LYLGNLPQTFESK</t>
+  </si>
+  <si>
+    <t>QTLAMQLNEK</t>
+  </si>
+  <si>
+    <t>WAVAEVLSNSPK</t>
+  </si>
+  <si>
+    <t>AYTALLDLKPGDNFELK</t>
+  </si>
+  <si>
+    <t>DMSPQALNEYK</t>
+  </si>
+  <si>
+    <t>GFQGSNGSLFR</t>
+  </si>
+  <si>
+    <t>LGTDAGMLAFEPSTVNLSAGDTVK</t>
+  </si>
+  <si>
+    <t>MLTGSDLLTK</t>
+  </si>
+  <si>
+    <t>ALQEAFQLR</t>
+  </si>
+  <si>
+    <t>TDEEGQSLLR</t>
+  </si>
+  <si>
+    <t>TFRPYTPGTR</t>
+  </si>
+  <si>
+    <t>YLSYALLAGDPSVLDDR</t>
+  </si>
+  <si>
+    <t>ACPLDVLEMVPWDGHK</t>
+  </si>
+  <si>
+    <t>AMLPVYESK</t>
+  </si>
+  <si>
+    <t>AQVFELPTGGAAEMNEGENLMYFAR</t>
+  </si>
+  <si>
+    <t>DLGDADLSGSYFSVSNLQK</t>
+  </si>
+  <si>
+    <t>EAAVADPANFDPR</t>
+  </si>
+  <si>
+    <t>EAGFELTADEVK</t>
+  </si>
+  <si>
+    <t>LLNYCLVTGGTGPLDELALNGQR</t>
+  </si>
+  <si>
+    <t>SYFPYWK</t>
+  </si>
+  <si>
+    <t>AELDYATK</t>
+  </si>
+  <si>
+    <t>AGSTLNLDTLVK</t>
+  </si>
+  <si>
+    <t>ANSFDDNK</t>
+  </si>
+  <si>
+    <t>FADVVNTGK</t>
+  </si>
+  <si>
+    <t>LLESLAPGLLK</t>
+  </si>
+  <si>
+    <t>QWFLVDAENQTLGR</t>
+  </si>
+  <si>
+    <t>SNQPLVNEK</t>
+  </si>
+  <si>
+    <t>SPLANLVGWR</t>
+  </si>
+  <si>
+    <t>SYVAAGNK</t>
+  </si>
+  <si>
+    <t>TCSLPLDR</t>
+  </si>
+  <si>
+    <t>AVVSADAK</t>
+  </si>
+  <si>
+    <t>DTGVEYAQGLVALGGDDEELAK</t>
+  </si>
+  <si>
+    <t>ETPVELEFSQLTK</t>
+  </si>
+  <si>
+    <t>LLAQAFGLLNER</t>
+  </si>
+  <si>
+    <t>YDSLLGQLK</t>
+  </si>
+  <si>
+    <t>GEELELVGLR</t>
+  </si>
+  <si>
+    <t>GFGSFEPR</t>
+  </si>
+  <si>
+    <t>NVQATLQR</t>
+  </si>
+  <si>
+    <t>VVTDFSEVTGR</t>
+  </si>
+  <si>
+    <t>YGCVAGYPSGSYLGNR</t>
+  </si>
+  <si>
+    <t>ADDEQTEENWEE</t>
+  </si>
+  <si>
+    <t>EFTVVNVAALNELK</t>
+  </si>
+  <si>
+    <t>LVPAGAEDSDD</t>
+  </si>
+  <si>
+    <t>LVVGGPYASVSDASSVLDASQK</t>
+  </si>
+  <si>
+    <t>QAGEYTTFK</t>
+  </si>
+  <si>
+    <t>FNPGLS</t>
+  </si>
+  <si>
+    <t>TDGLEVLSVADAAAK</t>
+  </si>
+  <si>
+    <t>TEFDVVLEGFDAAAK</t>
+  </si>
+  <si>
+    <t>TVTSASWR</t>
+  </si>
+  <si>
+    <t>FADLDVSK</t>
+  </si>
+  <si>
+    <t>FGNLVNTGR</t>
+  </si>
+  <si>
+    <t>LFLSPVESVLR</t>
+  </si>
+  <si>
+    <t>LGSDSGMLAFEPSSLTLQEGDTLK</t>
+  </si>
+  <si>
+    <t>TGSTLNLDTLVK</t>
+  </si>
+  <si>
+    <t>ACGYVSTK</t>
+  </si>
+  <si>
+    <t>DAFLYYPLQYEAQECSNNLFYTGATPNQQSEPATK</t>
+  </si>
+  <si>
+    <t>MLLSDLEGVTYR</t>
+  </si>
+  <si>
+    <t>YQWDQNFYR</t>
+  </si>
+  <si>
+    <t>ELELDDPFENLGAK</t>
+  </si>
+  <si>
+    <t>GLVPALEAADA</t>
+  </si>
+  <si>
+    <t>LLDQDEVPVVFGGWTSASR</t>
+  </si>
+  <si>
+    <t>QTQAAAPVAASAEEQK</t>
+  </si>
+  <si>
+    <t>SGEPYER</t>
+  </si>
+  <si>
+    <t>TVYVVSDSQLEELK</t>
+  </si>
+  <si>
+    <t>DLNALGFSDK</t>
   </si>
 </sst>
 </file>
@@ -1758,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F8545A-13E4-384E-A901-CD63BD0C8560}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1845,6 +2157,9 @@
       <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="H2" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1862,6 +2177,9 @@
       <c r="G3" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="H3" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1876,6 +2194,9 @@
       <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="H4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1890,6 +2211,9 @@
       <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="H5" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1901,6 +2225,9 @@
       <c r="G6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="H6" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -1912,6 +2239,9 @@
       <c r="G7" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H7" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -1920,70 +2250,532 @@
       <c r="G8" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="H8" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="H9" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G10" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="H10" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G11" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="H11" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G12" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="H12" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G13" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="H13" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="H14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G15" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="H15" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G16" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G18" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G20" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G21" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="H21" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="30" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="31" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="32" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="40" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="41" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="42" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="43" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="45" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="46" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="47" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="48" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="57" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="60" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="61" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="62" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="63" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H68" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="69" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="70" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="71" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="72" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="73" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="74" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="75" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="76" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="79" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="80" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="84" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="85" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="94" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="97" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="98" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="99" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="100" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="101" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="102" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="103" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="104" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="105" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>557</v>
       </c>
     </row>
   </sheetData>
@@ -1999,8 +2791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39D6E-ADCE-C54E-86E3-C5932C98575B}">
   <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2074,7 +2866,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B2" t="s">
         <v>150</v>
@@ -2092,13 +2884,13 @@
         <v>360</v>
       </c>
       <c r="G2" t="s">
-        <v>99</v>
+        <v>267</v>
       </c>
       <c r="H2" t="s">
         <v>125</v>
       </c>
       <c r="I2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="J2" t="s">
         <v>63</v>
@@ -2107,7 +2899,7 @@
         <v>63</v>
       </c>
       <c r="L2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M2" t="s">
         <v>86</v>
@@ -2116,7 +2908,7 @@
         <v>64</v>
       </c>
       <c r="O2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="P2" s="2" t="s">
         <v>48</v>
@@ -2124,31 +2916,31 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>164</v>
       </c>
       <c r="C3" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="D3" t="s">
-        <v>100</v>
+        <v>216</v>
       </c>
       <c r="E3" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="F3" t="s">
-        <v>361</v>
+        <v>409</v>
       </c>
       <c r="G3" t="s">
-        <v>100</v>
+        <v>409</v>
       </c>
       <c r="H3" t="s">
         <v>126</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="J3" t="s">
         <v>80</v>
@@ -2157,16 +2949,16 @@
         <v>66</v>
       </c>
       <c r="L3" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" t="s">
         <v>86</v>
       </c>
-      <c r="M3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N3" t="s">
-        <v>94</v>
-      </c>
       <c r="O3" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="P3" s="2" t="s">
         <v>49</v>
@@ -2174,46 +2966,46 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="E4" t="s">
-        <v>245</v>
+        <v>289</v>
       </c>
       <c r="F4" t="s">
-        <v>362</v>
+        <v>396</v>
       </c>
       <c r="G4" t="s">
-        <v>101</v>
+        <v>216</v>
       </c>
       <c r="H4" t="s">
         <v>127</v>
       </c>
       <c r="I4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="M4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="N4" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="O4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="P4" s="2" t="s">
         <v>49</v>
@@ -2221,40 +3013,40 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>191</v>
       </c>
       <c r="D5" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="E5" t="s">
-        <v>246</v>
+        <v>298</v>
       </c>
       <c r="F5" t="s">
-        <v>363</v>
+        <v>375</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>213</v>
       </c>
       <c r="H5" t="s">
         <v>128</v>
       </c>
       <c r="I5" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="J5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P5" s="2" t="s">
         <v>50</v>
@@ -2262,34 +3054,34 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="C6" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>225</v>
       </c>
       <c r="E6" t="s">
-        <v>247</v>
+        <v>278</v>
       </c>
       <c r="F6" t="s">
-        <v>364</v>
+        <v>382</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>396</v>
       </c>
       <c r="H6" t="s">
         <v>129</v>
       </c>
       <c r="I6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>51</v>
@@ -2297,34 +3089,34 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C7" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E7" t="s">
-        <v>248</v>
+        <v>284</v>
       </c>
       <c r="F7" t="s">
-        <v>365</v>
+        <v>376</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>221</v>
       </c>
       <c r="H7" t="s">
         <v>130</v>
       </c>
       <c r="I7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="O7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>52</v>
@@ -2332,34 +3124,34 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D8" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
-        <v>249</v>
+        <v>265</v>
       </c>
       <c r="F8" t="s">
-        <v>366</v>
+        <v>406</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>289</v>
       </c>
       <c r="H8" t="s">
         <v>57</v>
       </c>
       <c r="I8" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="O8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>53</v>
@@ -2367,34 +3159,34 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="B9" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C9" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D9" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="E9" t="s">
-        <v>250</v>
+        <v>293</v>
       </c>
       <c r="F9" t="s">
-        <v>367</v>
+        <v>415</v>
       </c>
       <c r="G9" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="H9" t="s">
         <v>131</v>
       </c>
       <c r="I9" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="O9" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>54</v>
@@ -2402,34 +3194,34 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D10" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E10" t="s">
-        <v>251</v>
+        <v>300</v>
       </c>
       <c r="F10" t="s">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c r="G10" t="s">
-        <v>107</v>
+        <v>194</v>
       </c>
       <c r="H10" t="s">
         <v>132</v>
       </c>
       <c r="I10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="O10" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>55</v>
@@ -2437,34 +3229,34 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="C11" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E11" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F11" t="s">
-        <v>369</v>
+        <v>388</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>225</v>
       </c>
       <c r="H11" t="s">
         <v>133</v>
       </c>
       <c r="I11" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="O11" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>56</v>
@@ -2472,34 +3264,34 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="C12" t="s">
         <v>195</v>
       </c>
       <c r="D12" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="E12" t="s">
-        <v>253</v>
+        <v>290</v>
       </c>
       <c r="F12" t="s">
-        <v>370</v>
+        <v>399</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>164</v>
       </c>
       <c r="H12" t="s">
         <v>134</v>
       </c>
       <c r="I12" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="O12" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="P12" s="2" t="s">
         <v>57</v>
@@ -2507,34 +3299,34 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="C13" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D13" t="s">
         <v>218</v>
       </c>
       <c r="E13" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="F13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="G13" t="s">
-        <v>110</v>
+        <v>278</v>
       </c>
       <c r="H13" t="s">
         <v>135</v>
       </c>
       <c r="I13" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="O13" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="P13" s="2" t="s">
         <v>58</v>
@@ -2542,34 +3334,34 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B14" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C14" t="s">
-        <v>197</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="E14" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="F14" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
       <c r="G14" t="s">
-        <v>111</v>
+        <v>209</v>
       </c>
       <c r="H14" t="s">
         <v>136</v>
       </c>
       <c r="I14" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="O14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>59</v>
@@ -2577,31 +3369,31 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="E15" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="F15" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="G15" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
       <c r="H15" t="s">
         <v>137</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="O15" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>49</v>
@@ -2609,31 +3401,31 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D16" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="E16" t="s">
-        <v>257</v>
+        <v>285</v>
       </c>
       <c r="F16" t="s">
-        <v>100</v>
+        <v>368</v>
       </c>
       <c r="G16" t="s">
-        <v>113</v>
+        <v>170</v>
       </c>
       <c r="H16" t="s">
         <v>138</v>
       </c>
       <c r="I16" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="O16" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>60</v>
@@ -2641,31 +3433,31 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D17" t="s">
+        <v>219</v>
+      </c>
+      <c r="E17" t="s">
+        <v>291</v>
+      </c>
+      <c r="F17" t="s">
+        <v>379</v>
+      </c>
+      <c r="G17" t="s">
         <v>222</v>
-      </c>
-      <c r="E17" t="s">
-        <v>258</v>
-      </c>
-      <c r="F17" t="s">
-        <v>374</v>
-      </c>
-      <c r="G17" t="s">
-        <v>114</v>
       </c>
       <c r="H17" t="s">
         <v>139</v>
       </c>
       <c r="I17" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="O17" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>49</v>
@@ -2673,31 +3465,31 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="B18" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D18" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="E18" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="F18" t="s">
-        <v>375</v>
+        <v>404</v>
       </c>
       <c r="G18" t="s">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="H18" t="s">
         <v>140</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>49</v>
@@ -2705,31 +3497,31 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D19" t="s">
-        <v>224</v>
+        <v>100</v>
       </c>
       <c r="E19" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="F19" t="s">
-        <v>376</v>
+        <v>403</v>
       </c>
       <c r="G19" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="H19" t="s">
         <v>141</v>
       </c>
       <c r="I19" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="O19" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="P19" s="2" t="s">
         <v>61</v>
@@ -2737,28 +3529,28 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="D20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="E20" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="F20" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
       <c r="G20" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="H20" t="s">
         <v>142</v>
       </c>
       <c r="O20" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="P20" t="s">
         <v>49</v>
@@ -2766,28 +3558,28 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D21" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="E21" t="s">
-        <v>262</v>
+        <v>296</v>
       </c>
       <c r="F21" t="s">
-        <v>378</v>
+        <v>411</v>
       </c>
       <c r="G21" t="s">
-        <v>118</v>
+        <v>284</v>
       </c>
       <c r="H21" t="s">
         <v>143</v>
       </c>
       <c r="O21" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="P21" t="s">
         <v>83</v>
@@ -2795,25 +3587,25 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>263</v>
+        <v>302</v>
       </c>
       <c r="F22" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
       <c r="G22" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="H22" t="s">
         <v>144</v>
       </c>
       <c r="O22" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="P22" t="s">
         <v>84</v>
@@ -2821,25 +3613,25 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B23" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="E23" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="F23" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="G23" t="s">
-        <v>120</v>
+        <v>265</v>
       </c>
       <c r="H23" t="s">
         <v>145</v>
       </c>
       <c r="O23" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="P23" t="s">
         <v>85</v>
@@ -2847,22 +3639,22 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="E24" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="F24" t="s">
-        <v>381</v>
+        <v>113</v>
       </c>
       <c r="G24" t="s">
-        <v>121</v>
+        <v>293</v>
       </c>
       <c r="H24" t="s">
         <v>146</v>
       </c>
       <c r="O24" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="P24" t="s">
         <v>49</v>
@@ -2870,22 +3662,22 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>266</v>
+        <v>303</v>
       </c>
       <c r="F25" t="s">
-        <v>382</v>
+        <v>395</v>
       </c>
       <c r="G25" t="s">
-        <v>122</v>
+        <v>375</v>
       </c>
       <c r="H25" t="s">
         <v>147</v>
       </c>
       <c r="O25" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P25" t="s">
         <v>51</v>
@@ -2893,22 +3685,22 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="E26" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="F26" t="s">
-        <v>383</v>
+        <v>417</v>
       </c>
       <c r="G26" t="s">
-        <v>123</v>
+        <v>382</v>
       </c>
       <c r="H26" t="s">
         <v>148</v>
       </c>
       <c r="O26" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="P26" t="s">
         <v>90</v>
@@ -2916,22 +3708,22 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="E27" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="F27" t="s">
-        <v>163</v>
+        <v>380</v>
       </c>
       <c r="G27" t="s">
-        <v>124</v>
+        <v>376</v>
       </c>
       <c r="H27" t="s">
         <v>149</v>
       </c>
       <c r="O27" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="P27" t="s">
         <v>91</v>
@@ -2939,19 +3731,19 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
-        <v>269</v>
+        <v>292</v>
       </c>
       <c r="F28" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="G28" t="s">
-        <v>150</v>
+        <v>191</v>
       </c>
       <c r="H28" t="s">
         <v>171</v>
       </c>
       <c r="O28" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="P28" t="s">
         <v>92</v>
@@ -2959,19 +3751,19 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="F29" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G29" t="s">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="H29" t="s">
         <v>126</v>
       </c>
       <c r="O29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="P29" t="s">
         <v>93</v>
@@ -2979,13 +3771,13 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E30" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="F30" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="G30" t="s">
-        <v>151</v>
+        <v>193</v>
       </c>
       <c r="H30" t="s">
         <v>53</v>
@@ -2999,19 +3791,19 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E31" t="s">
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="F31" t="s">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="G31" t="s">
-        <v>152</v>
+        <v>118</v>
       </c>
       <c r="H31" t="s">
         <v>172</v>
       </c>
       <c r="O31" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="P31" t="s">
         <v>95</v>
@@ -3019,19 +3811,19 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="E32" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="F32" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
       <c r="G32" t="s">
-        <v>153</v>
+        <v>300</v>
       </c>
       <c r="H32" t="s">
         <v>53</v>
       </c>
       <c r="O32" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="P32" t="s">
         <v>90</v>
@@ -3039,19 +3831,19 @@
     </row>
     <row r="33" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E33" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="F33" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="G33" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="H33" t="s">
         <v>173</v>
       </c>
       <c r="O33" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="P33" t="s">
         <v>91</v>
@@ -3059,19 +3851,19 @@
     </row>
     <row r="34" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E34" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="F34" t="s">
-        <v>113</v>
+        <v>371</v>
       </c>
       <c r="G34" t="s">
-        <v>155</v>
+        <v>253</v>
       </c>
       <c r="H34" t="s">
         <v>174</v>
       </c>
       <c r="O34" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="P34" t="s">
         <v>90</v>
@@ -3079,19 +3871,19 @@
     </row>
     <row r="35" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E35" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="F35" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="G35" t="s">
-        <v>156</v>
+        <v>290</v>
       </c>
       <c r="H35" t="s">
         <v>57</v>
       </c>
       <c r="O35" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="P35" t="s">
         <v>97</v>
@@ -3099,13 +3891,13 @@
     </row>
     <row r="36" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E36" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="F36" t="s">
         <v>391</v>
       </c>
       <c r="G36" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
       <c r="H36" t="s">
         <v>175</v>
@@ -3113,13 +3905,13 @@
     </row>
     <row r="37" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E37" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="F37" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="G37" t="s">
-        <v>158</v>
+        <v>406</v>
       </c>
       <c r="H37" t="s">
         <v>176</v>
@@ -3127,13 +3919,13 @@
     </row>
     <row r="38" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E38" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="F38" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="G38" t="s">
-        <v>159</v>
+        <v>223</v>
       </c>
       <c r="H38" t="s">
         <v>177</v>
@@ -3141,13 +3933,13 @@
     </row>
     <row r="39" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E39" t="s">
-        <v>280</v>
+        <v>294</v>
       </c>
       <c r="F39" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="G39" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H39" t="s">
         <v>128</v>
@@ -3155,13 +3947,13 @@
     </row>
     <row r="40" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E40" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="F40" t="s">
-        <v>395</v>
+        <v>364</v>
       </c>
       <c r="G40" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H40" t="s">
         <v>178</v>
@@ -3169,13 +3961,13 @@
     </row>
     <row r="41" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E41" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
       <c r="F41" t="s">
-        <v>396</v>
+        <v>407</v>
       </c>
       <c r="G41" t="s">
-        <v>162</v>
+        <v>217</v>
       </c>
       <c r="H41" t="s">
         <v>49</v>
@@ -3183,13 +3975,13 @@
     </row>
     <row r="42" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
-        <v>283</v>
+        <v>305</v>
       </c>
       <c r="F42" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="G42" t="s">
-        <v>163</v>
+        <v>415</v>
       </c>
       <c r="H42" t="s">
         <v>179</v>
@@ -3197,13 +3989,13 @@
     </row>
     <row r="43" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E43" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F43" t="s">
-        <v>398</v>
+        <v>372</v>
       </c>
       <c r="G43" t="s">
-        <v>164</v>
+        <v>400</v>
       </c>
       <c r="H43" t="s">
         <v>180</v>
@@ -3211,13 +4003,13 @@
     </row>
     <row r="44" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E44" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="F44" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G44" t="s">
-        <v>165</v>
+        <v>388</v>
       </c>
       <c r="H44" t="s">
         <v>181</v>
@@ -3225,13 +4017,13 @@
     </row>
     <row r="45" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E45" t="s">
-        <v>286</v>
+        <v>251</v>
       </c>
       <c r="F45" t="s">
-        <v>400</v>
+        <v>163</v>
       </c>
       <c r="G45" t="s">
-        <v>166</v>
+        <v>106</v>
       </c>
       <c r="H45" t="s">
         <v>182</v>
@@ -3239,13 +4031,13 @@
     </row>
     <row r="46" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E46" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="F46" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="G46" t="s">
-        <v>167</v>
+        <v>399</v>
       </c>
       <c r="H46" t="s">
         <v>183</v>
@@ -3253,13 +4045,13 @@
     </row>
     <row r="47" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E47" t="s">
-        <v>288</v>
+        <v>254</v>
       </c>
       <c r="F47" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="G47" t="s">
-        <v>168</v>
+        <v>370</v>
       </c>
       <c r="H47" t="s">
         <v>53</v>
@@ -3267,13 +4059,13 @@
     </row>
     <row r="48" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E48" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="F48" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="G48" t="s">
-        <v>169</v>
+        <v>214</v>
       </c>
       <c r="H48" t="s">
         <v>184</v>
@@ -3281,13 +4073,13 @@
     </row>
     <row r="49" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E49" t="s">
-        <v>290</v>
+        <v>263</v>
       </c>
       <c r="F49" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="G49" t="s">
-        <v>170</v>
+        <v>196</v>
       </c>
       <c r="H49" t="s">
         <v>185</v>
@@ -3295,13 +4087,13 @@
     </row>
     <row r="50" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E50" t="s">
-        <v>291</v>
+        <v>269</v>
       </c>
       <c r="F50" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
       <c r="G50" t="s">
-        <v>186</v>
+        <v>360</v>
       </c>
       <c r="H50" t="s">
         <v>198</v>
@@ -3309,13 +4101,13 @@
     </row>
     <row r="51" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E51" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="F51" t="s">
-        <v>406</v>
+        <v>369</v>
       </c>
       <c r="G51" t="s">
-        <v>187</v>
+        <v>378</v>
       </c>
       <c r="H51" t="s">
         <v>199</v>
@@ -3323,13 +4115,13 @@
     </row>
     <row r="52" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E52" t="s">
-        <v>293</v>
+        <v>247</v>
       </c>
       <c r="F52" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="G52" t="s">
-        <v>188</v>
+        <v>260</v>
       </c>
       <c r="H52" t="s">
         <v>200</v>
@@ -3337,13 +4129,13 @@
     </row>
     <row r="53" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E53" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="F53" t="s">
-        <v>408</v>
+        <v>366</v>
       </c>
       <c r="G53" t="s">
-        <v>100</v>
+        <v>361</v>
       </c>
       <c r="H53" t="s">
         <v>126</v>
@@ -3351,13 +4143,13 @@
     </row>
     <row r="54" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E54" t="s">
-        <v>295</v>
+        <v>306</v>
       </c>
       <c r="F54" t="s">
-        <v>409</v>
+        <v>374</v>
       </c>
       <c r="G54" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H54" t="s">
         <v>201</v>
@@ -3365,13 +4157,13 @@
     </row>
     <row r="55" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E55" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F55" t="s">
-        <v>410</v>
+        <v>100</v>
       </c>
       <c r="G55" t="s">
-        <v>190</v>
+        <v>368</v>
       </c>
       <c r="H55" t="s">
         <v>92</v>
@@ -3379,13 +4171,13 @@
     </row>
     <row r="56" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E56" t="s">
-        <v>297</v>
+        <v>252</v>
       </c>
       <c r="F56" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="G56" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H56" t="s">
         <v>53</v>
@@ -3393,13 +4185,13 @@
     </row>
     <row r="57" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E57" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="F57" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="G57" t="s">
-        <v>192</v>
+        <v>379</v>
       </c>
       <c r="H57" t="s">
         <v>202</v>
@@ -3407,13 +4199,13 @@
     </row>
     <row r="58" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E58" t="s">
-        <v>299</v>
+        <v>271</v>
       </c>
       <c r="F58" t="s">
-        <v>413</v>
+        <v>365</v>
       </c>
       <c r="G58" t="s">
-        <v>193</v>
+        <v>404</v>
       </c>
       <c r="H58" t="s">
         <v>203</v>
@@ -3421,13 +4213,13 @@
     </row>
     <row r="59" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E59" t="s">
-        <v>300</v>
+        <v>270</v>
       </c>
       <c r="F59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="G59" t="s">
-        <v>194</v>
+        <v>403</v>
       </c>
       <c r="H59" t="s">
         <v>204</v>
@@ -3435,13 +4227,13 @@
     </row>
     <row r="60" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E60" t="s">
-        <v>301</v>
+        <v>264</v>
       </c>
       <c r="F60" t="s">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="G60" t="s">
-        <v>195</v>
+        <v>363</v>
       </c>
       <c r="H60" t="s">
         <v>205</v>
@@ -3449,13 +4241,13 @@
     </row>
     <row r="61" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E61" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="F61" t="s">
-        <v>416</v>
+        <v>367</v>
       </c>
       <c r="G61" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="H61" t="s">
         <v>206</v>
@@ -3463,13 +4255,13 @@
     </row>
     <row r="62" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E62" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
       <c r="F62" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
       <c r="G62" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="H62" t="s">
         <v>207</v>
@@ -3477,10 +4269,10 @@
     </row>
     <row r="63" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E63" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="G63" t="s">
-        <v>208</v>
+        <v>262</v>
       </c>
       <c r="H63" t="s">
         <v>227</v>
@@ -3488,10 +4280,10 @@
     </row>
     <row r="64" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E64" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="G64" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="H64" t="s">
         <v>126</v>
@@ -3499,10 +4291,10 @@
     </row>
     <row r="65" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E65" t="s">
-        <v>306</v>
+        <v>244</v>
       </c>
       <c r="G65" t="s">
-        <v>209</v>
+        <v>285</v>
       </c>
       <c r="H65" t="s">
         <v>228</v>
@@ -3510,10 +4302,10 @@
     </row>
     <row r="66" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E66" t="s">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="G66" t="s">
-        <v>210</v>
+        <v>105</v>
       </c>
       <c r="H66" t="s">
         <v>229</v>
@@ -3521,10 +4313,10 @@
     </row>
     <row r="67" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E67" t="s">
-        <v>308</v>
+        <v>273</v>
       </c>
       <c r="G67" t="s">
-        <v>211</v>
+        <v>291</v>
       </c>
       <c r="H67" t="s">
         <v>230</v>
@@ -3532,10 +4324,10 @@
     </row>
     <row r="68" spans="5:8" x14ac:dyDescent="0.2">
       <c r="E68" t="s">
-        <v>309</v>
+        <v>276</v>
       </c>
       <c r="G68" t="s">
-        <v>212</v>
+        <v>188</v>
       </c>
       <c r="H68" t="s">
         <v>231</v>
@@ -3543,7 +4335,7 @@
     </row>
     <row r="69" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G69" t="s">
-        <v>213</v>
+        <v>309</v>
       </c>
       <c r="H69" t="s">
         <v>232</v>
@@ -3551,7 +4343,7 @@
     </row>
     <row r="70" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G70" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="H70" t="s">
         <v>83</v>
@@ -3559,7 +4351,7 @@
     </row>
     <row r="71" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G71" t="s">
-        <v>215</v>
+        <v>411</v>
       </c>
       <c r="H71" t="s">
         <v>233</v>
@@ -3567,7 +4359,7 @@
     </row>
     <row r="72" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G72" t="s">
-        <v>216</v>
+        <v>257</v>
       </c>
       <c r="H72" t="s">
         <v>234</v>
@@ -3575,7 +4367,7 @@
     </row>
     <row r="73" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G73" t="s">
-        <v>217</v>
+        <v>387</v>
       </c>
       <c r="H73" t="s">
         <v>207</v>
@@ -3583,7 +4375,7 @@
     </row>
     <row r="74" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G74" t="s">
-        <v>218</v>
+        <v>119</v>
       </c>
       <c r="H74" t="s">
         <v>235</v>
@@ -3591,7 +4383,7 @@
     </row>
     <row r="75" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G75" t="s">
-        <v>219</v>
+        <v>272</v>
       </c>
       <c r="H75" t="s">
         <v>236</v>
@@ -3599,7 +4391,7 @@
     </row>
     <row r="76" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G76" t="s">
-        <v>220</v>
+        <v>296</v>
       </c>
       <c r="H76" t="s">
         <v>237</v>
@@ -3607,7 +4399,7 @@
     </row>
     <row r="77" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G77" t="s">
-        <v>221</v>
+        <v>115</v>
       </c>
       <c r="H77" t="s">
         <v>238</v>
@@ -3615,7 +4407,7 @@
     </row>
     <row r="78" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G78" t="s">
-        <v>222</v>
+        <v>168</v>
       </c>
       <c r="H78" t="s">
         <v>239</v>
@@ -3623,7 +4415,7 @@
     </row>
     <row r="79" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G79" t="s">
-        <v>223</v>
+        <v>302</v>
       </c>
       <c r="H79" t="s">
         <v>240</v>
@@ -3631,7 +4423,7 @@
     </row>
     <row r="80" spans="5:8" x14ac:dyDescent="0.2">
       <c r="G80" t="s">
-        <v>224</v>
+        <v>362</v>
       </c>
       <c r="H80" t="s">
         <v>241</v>
@@ -3639,7 +4431,7 @@
     </row>
     <row r="81" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G81" t="s">
-        <v>225</v>
+        <v>243</v>
       </c>
       <c r="H81" t="s">
         <v>242</v>
@@ -3647,7 +4439,7 @@
     </row>
     <row r="82" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G82" t="s">
-        <v>226</v>
+        <v>110</v>
       </c>
       <c r="H82" t="s">
         <v>198</v>
@@ -3655,7 +4447,7 @@
     </row>
     <row r="83" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G83" t="s">
-        <v>243</v>
+        <v>113</v>
       </c>
       <c r="H83" t="s">
         <v>310</v>
@@ -3663,7 +4455,7 @@
     </row>
     <row r="84" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G84" t="s">
-        <v>244</v>
+        <v>113</v>
       </c>
       <c r="H84" t="s">
         <v>311</v>
@@ -3671,7 +4463,7 @@
     </row>
     <row r="85" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G85" t="s">
-        <v>245</v>
+        <v>114</v>
       </c>
       <c r="H85" t="s">
         <v>312</v>
@@ -3679,7 +4471,7 @@
     </row>
     <row r="86" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G86" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="H86" t="s">
         <v>313</v>
@@ -3687,7 +4479,7 @@
     </row>
     <row r="87" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G87" t="s">
-        <v>247</v>
+        <v>107</v>
       </c>
       <c r="H87" t="s">
         <v>314</v>
@@ -3695,7 +4487,7 @@
     </row>
     <row r="88" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G88" t="s">
-        <v>248</v>
+        <v>395</v>
       </c>
       <c r="H88" t="s">
         <v>315</v>
@@ -3703,7 +4495,7 @@
     </row>
     <row r="89" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G89" t="s">
-        <v>249</v>
+        <v>274</v>
       </c>
       <c r="H89" t="s">
         <v>53</v>
@@ -3711,7 +4503,7 @@
     </row>
     <row r="90" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G90" t="s">
-        <v>250</v>
+        <v>116</v>
       </c>
       <c r="H90" t="s">
         <v>59</v>
@@ -3719,7 +4511,7 @@
     </row>
     <row r="91" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G91" t="s">
-        <v>251</v>
+        <v>112</v>
       </c>
       <c r="H91" t="s">
         <v>49</v>
@@ -3727,7 +4519,7 @@
     </row>
     <row r="92" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G92" t="s">
-        <v>252</v>
+        <v>218</v>
       </c>
       <c r="H92" t="s">
         <v>316</v>
@@ -3735,7 +4527,7 @@
     </row>
     <row r="93" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G93" t="s">
-        <v>253</v>
+        <v>417</v>
       </c>
       <c r="H93" t="s">
         <v>317</v>
@@ -3743,7 +4535,7 @@
     </row>
     <row r="94" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G94" t="s">
-        <v>254</v>
+        <v>303</v>
       </c>
       <c r="H94" t="s">
         <v>318</v>
@@ -3751,7 +4543,7 @@
     </row>
     <row r="95" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G95" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H95" t="s">
         <v>319</v>
@@ -3759,7 +4551,7 @@
     </row>
     <row r="96" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G96" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="H96" t="s">
         <v>320</v>
@@ -3767,7 +4559,7 @@
     </row>
     <row r="97" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G97" t="s">
-        <v>257</v>
+        <v>154</v>
       </c>
       <c r="H97" t="s">
         <v>314</v>
@@ -3775,7 +4567,7 @@
     </row>
     <row r="98" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G98" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="H98" t="s">
         <v>321</v>
@@ -3783,7 +4575,7 @@
     </row>
     <row r="99" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G99" t="s">
-        <v>259</v>
+        <v>380</v>
       </c>
       <c r="H99" t="s">
         <v>57</v>
@@ -3791,7 +4583,7 @@
     </row>
     <row r="100" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G100" t="s">
-        <v>260</v>
+        <v>152</v>
       </c>
       <c r="H100" t="s">
         <v>322</v>
@@ -3799,7 +4591,7 @@
     </row>
     <row r="101" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G101" t="s">
-        <v>261</v>
+        <v>373</v>
       </c>
       <c r="H101" t="s">
         <v>323</v>
@@ -3807,7 +4599,7 @@
     </row>
     <row r="102" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G102" t="s">
-        <v>262</v>
+        <v>165</v>
       </c>
       <c r="H102" t="s">
         <v>324</v>
@@ -3815,7 +4607,7 @@
     </row>
     <row r="103" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G103" t="s">
-        <v>263</v>
+        <v>384</v>
       </c>
       <c r="H103" t="s">
         <v>325</v>
@@ -3823,7 +4615,7 @@
     </row>
     <row r="104" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G104" t="s">
-        <v>264</v>
+        <v>282</v>
       </c>
       <c r="H104" t="s">
         <v>326</v>
@@ -3831,7 +4623,7 @@
     </row>
     <row r="105" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G105" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H105" t="s">
         <v>327</v>
@@ -3839,7 +4631,7 @@
     </row>
     <row r="106" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G106" t="s">
-        <v>266</v>
+        <v>304</v>
       </c>
       <c r="H106" t="s">
         <v>207</v>
@@ -3847,7 +4639,7 @@
     </row>
     <row r="107" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G107" t="s">
-        <v>267</v>
+        <v>393</v>
       </c>
       <c r="H107" t="s">
         <v>233</v>
@@ -3855,7 +4647,7 @@
     </row>
     <row r="108" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G108" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="H108" t="s">
         <v>328</v>
@@ -3863,7 +4655,7 @@
     </row>
     <row r="109" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G109" t="s">
-        <v>269</v>
+        <v>190</v>
       </c>
       <c r="H109" t="s">
         <v>329</v>
@@ -3871,7 +4663,7 @@
     </row>
     <row r="110" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G110" t="s">
-        <v>270</v>
+        <v>397</v>
       </c>
       <c r="H110" t="s">
         <v>330</v>
@@ -3879,7 +4671,7 @@
     </row>
     <row r="111" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G111" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H111" t="s">
         <v>49</v>
@@ -3887,7 +4679,7 @@
     </row>
     <row r="112" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G112" t="s">
-        <v>272</v>
+        <v>280</v>
       </c>
       <c r="H112" t="s">
         <v>331</v>
@@ -3895,7 +4687,7 @@
     </row>
     <row r="113" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G113" t="s">
-        <v>273</v>
+        <v>414</v>
       </c>
       <c r="H113" t="s">
         <v>332</v>
@@ -3903,7 +4695,7 @@
     </row>
     <row r="114" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G114" t="s">
-        <v>274</v>
+        <v>299</v>
       </c>
       <c r="H114" t="s">
         <v>95</v>
@@ -3911,7 +4703,7 @@
     </row>
     <row r="115" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G115" t="s">
-        <v>275</v>
+        <v>390</v>
       </c>
       <c r="H115" t="s">
         <v>333</v>
@@ -3919,7 +4711,7 @@
     </row>
     <row r="116" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G116" t="s">
-        <v>276</v>
+        <v>371</v>
       </c>
       <c r="H116" t="s">
         <v>334</v>
@@ -3927,7 +4719,7 @@
     </row>
     <row r="117" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G117" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="H117" t="s">
         <v>316</v>
@@ -3935,7 +4727,7 @@
     </row>
     <row r="118" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G118" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="H118" t="s">
         <v>335</v>
@@ -3943,7 +4735,7 @@
     </row>
     <row r="119" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G119" t="s">
-        <v>279</v>
+        <v>120</v>
       </c>
       <c r="H119" t="s">
         <v>336</v>
@@ -3951,7 +4743,7 @@
     </row>
     <row r="120" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G120" t="s">
-        <v>280</v>
+        <v>383</v>
       </c>
       <c r="H120" t="s">
         <v>337</v>
@@ -3967,7 +4759,7 @@
     </row>
     <row r="122" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G122" t="s">
-        <v>282</v>
+        <v>391</v>
       </c>
       <c r="H122" t="s">
         <v>339</v>
@@ -3975,7 +4767,7 @@
     </row>
     <row r="123" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G123" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
       <c r="H123" t="s">
         <v>340</v>
@@ -3983,7 +4775,7 @@
     </row>
     <row r="124" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G124" t="s">
-        <v>284</v>
+        <v>402</v>
       </c>
       <c r="H124" t="s">
         <v>341</v>
@@ -3991,7 +4783,7 @@
     </row>
     <row r="125" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G125" t="s">
-        <v>285</v>
+        <v>224</v>
       </c>
       <c r="H125" t="s">
         <v>59</v>
@@ -3999,7 +4791,7 @@
     </row>
     <row r="126" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G126" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="H126" t="s">
         <v>335</v>
@@ -4007,7 +4799,7 @@
     </row>
     <row r="127" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G127" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="H127" t="s">
         <v>233</v>
@@ -4015,7 +4807,7 @@
     </row>
     <row r="128" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G128" t="s">
-        <v>288</v>
+        <v>211</v>
       </c>
       <c r="H128" t="s">
         <v>342</v>
@@ -4023,7 +4815,7 @@
     </row>
     <row r="129" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G129" t="s">
-        <v>289</v>
+        <v>305</v>
       </c>
       <c r="H129" t="s">
         <v>56</v>
@@ -4031,7 +4823,7 @@
     </row>
     <row r="130" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G130" t="s">
-        <v>290</v>
+        <v>162</v>
       </c>
       <c r="H130" t="s">
         <v>343</v>
@@ -4039,7 +4831,7 @@
     </row>
     <row r="131" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G131" t="s">
-        <v>291</v>
+        <v>394</v>
       </c>
       <c r="H131" t="s">
         <v>344</v>
@@ -4047,7 +4839,7 @@
     </row>
     <row r="132" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G132" t="s">
-        <v>292</v>
+        <v>286</v>
       </c>
       <c r="H132" t="s">
         <v>345</v>
@@ -4055,7 +4847,7 @@
     </row>
     <row r="133" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G133" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="H133" t="s">
         <v>239</v>
@@ -4063,7 +4855,7 @@
     </row>
     <row r="134" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G134" t="s">
-        <v>294</v>
+        <v>386</v>
       </c>
       <c r="H134" t="s">
         <v>346</v>
@@ -4071,7 +4863,7 @@
     </row>
     <row r="135" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G135" t="s">
-        <v>295</v>
+        <v>99</v>
       </c>
       <c r="H135" t="s">
         <v>347</v>
@@ -4079,7 +4871,7 @@
     </row>
     <row r="136" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G136" t="s">
-        <v>296</v>
+        <v>124</v>
       </c>
       <c r="H136" t="s">
         <v>348</v>
@@ -4087,7 +4879,7 @@
     </row>
     <row r="137" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G137" t="s">
-        <v>297</v>
+        <v>195</v>
       </c>
       <c r="H137" t="s">
         <v>349</v>
@@ -4095,7 +4887,7 @@
     </row>
     <row r="138" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G138" t="s">
-        <v>298</v>
+        <v>251</v>
       </c>
       <c r="H138" t="s">
         <v>350</v>
@@ -4103,7 +4895,7 @@
     </row>
     <row r="139" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G139" t="s">
-        <v>299</v>
+        <v>364</v>
       </c>
       <c r="H139" t="s">
         <v>351</v>
@@ -4111,7 +4903,7 @@
     </row>
     <row r="140" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G140" t="s">
-        <v>300</v>
+        <v>208</v>
       </c>
       <c r="H140" t="s">
         <v>352</v>
@@ -4119,7 +4911,7 @@
     </row>
     <row r="141" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G141" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="H141" t="s">
         <v>353</v>
@@ -4127,7 +4919,7 @@
     </row>
     <row r="142" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G142" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="H142" t="s">
         <v>354</v>
@@ -4135,7 +4927,7 @@
     </row>
     <row r="143" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G143" t="s">
-        <v>303</v>
+        <v>103</v>
       </c>
       <c r="H143" t="s">
         <v>355</v>
@@ -4143,7 +4935,7 @@
     </row>
     <row r="144" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G144" t="s">
-        <v>304</v>
+        <v>279</v>
       </c>
       <c r="H144" t="s">
         <v>356</v>
@@ -4151,7 +4943,7 @@
     </row>
     <row r="145" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G145" t="s">
-        <v>305</v>
+        <v>263</v>
       </c>
       <c r="H145" t="s">
         <v>357</v>
@@ -4159,7 +4951,7 @@
     </row>
     <row r="146" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G146" t="s">
-        <v>306</v>
+        <v>407</v>
       </c>
       <c r="H146" t="s">
         <v>358</v>
@@ -4167,7 +4959,7 @@
     </row>
     <row r="147" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G147" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="H147" t="s">
         <v>53</v>
@@ -4175,7 +4967,7 @@
     </row>
     <row r="148" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G148" t="s">
-        <v>308</v>
+        <v>389</v>
       </c>
       <c r="H148" t="s">
         <v>322</v>
@@ -4183,7 +4975,7 @@
     </row>
     <row r="149" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G149" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="H149" t="s">
         <v>359</v>
@@ -4191,7 +4983,7 @@
     </row>
     <row r="150" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G150" t="s">
-        <v>360</v>
+        <v>372</v>
       </c>
       <c r="H150" t="s">
         <v>418</v>
@@ -4199,7 +4991,7 @@
     </row>
     <row r="151" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G151" t="s">
-        <v>361</v>
+        <v>247</v>
       </c>
       <c r="H151" t="s">
         <v>419</v>
@@ -4207,7 +4999,7 @@
     </row>
     <row r="152" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G152" t="s">
-        <v>362</v>
+        <v>246</v>
       </c>
       <c r="H152" t="s">
         <v>420</v>
@@ -4215,7 +5007,7 @@
     </row>
     <row r="153" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G153" t="s">
-        <v>363</v>
+        <v>212</v>
       </c>
       <c r="H153" t="s">
         <v>421</v>
@@ -4223,7 +5015,7 @@
     </row>
     <row r="154" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G154" t="s">
-        <v>364</v>
+        <v>306</v>
       </c>
       <c r="H154" t="s">
         <v>238</v>
@@ -4231,7 +5023,7 @@
     </row>
     <row r="155" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G155" t="s">
-        <v>365</v>
+        <v>219</v>
       </c>
       <c r="H155" t="s">
         <v>422</v>
@@ -4239,7 +5031,7 @@
     </row>
     <row r="156" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G156" t="s">
-        <v>366</v>
+        <v>157</v>
       </c>
       <c r="H156" t="s">
         <v>423</v>
@@ -4247,7 +5039,7 @@
     </row>
     <row r="157" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G157" t="s">
-        <v>367</v>
+        <v>283</v>
       </c>
       <c r="H157" t="s">
         <v>60</v>
@@ -4255,7 +5047,7 @@
     </row>
     <row r="158" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G158" t="s">
-        <v>368</v>
+        <v>252</v>
       </c>
       <c r="H158" t="s">
         <v>424</v>
@@ -4263,7 +5055,7 @@
     </row>
     <row r="159" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G159" t="s">
-        <v>369</v>
+        <v>158</v>
       </c>
       <c r="H159" t="s">
         <v>345</v>
@@ -4271,7 +5063,7 @@
     </row>
     <row r="160" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G160" t="s">
-        <v>370</v>
+        <v>295</v>
       </c>
       <c r="H160" t="s">
         <v>342</v>
@@ -4279,7 +5071,7 @@
     </row>
     <row r="161" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G161" t="s">
-        <v>371</v>
+        <v>401</v>
       </c>
       <c r="H161" t="s">
         <v>54</v>
@@ -4287,7 +5079,7 @@
     </row>
     <row r="162" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G162" t="s">
-        <v>372</v>
+        <v>271</v>
       </c>
       <c r="H162" t="s">
         <v>425</v>
@@ -4295,7 +5087,7 @@
     </row>
     <row r="163" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G163" t="s">
-        <v>373</v>
+        <v>163</v>
       </c>
       <c r="H163" t="s">
         <v>205</v>
@@ -4303,7 +5095,7 @@
     </row>
     <row r="164" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G164" t="s">
-        <v>100</v>
+        <v>163</v>
       </c>
       <c r="H164" t="s">
         <v>126</v>
@@ -4311,7 +5103,7 @@
     </row>
     <row r="165" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G165" t="s">
-        <v>374</v>
+        <v>408</v>
       </c>
       <c r="H165" t="s">
         <v>143</v>
@@ -4319,7 +5111,7 @@
     </row>
     <row r="166" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G166" t="s">
-        <v>375</v>
+        <v>405</v>
       </c>
       <c r="H166" t="s">
         <v>426</v>
@@ -4327,7 +5119,7 @@
     </row>
     <row r="167" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G167" t="s">
-        <v>376</v>
+        <v>220</v>
       </c>
       <c r="H167" t="s">
         <v>427</v>
@@ -4335,7 +5127,7 @@
     </row>
     <row r="168" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G168" t="s">
-        <v>377</v>
+        <v>410</v>
       </c>
       <c r="H168" t="s">
         <v>428</v>
@@ -4343,7 +5135,7 @@
     </row>
     <row r="169" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G169" t="s">
-        <v>378</v>
+        <v>398</v>
       </c>
       <c r="H169" t="s">
         <v>429</v>
@@ -4351,7 +5143,7 @@
     </row>
     <row r="170" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G170" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H170" t="s">
         <v>430</v>
@@ -4359,7 +5151,7 @@
     </row>
     <row r="171" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G171" t="s">
-        <v>380</v>
+        <v>160</v>
       </c>
       <c r="H171" t="s">
         <v>431</v>
@@ -4367,7 +5159,7 @@
     </row>
     <row r="172" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G172" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="H172" t="s">
         <v>139</v>
@@ -4375,7 +5167,7 @@
     </row>
     <row r="173" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G173" t="s">
-        <v>382</v>
+        <v>122</v>
       </c>
       <c r="H173" t="s">
         <v>432</v>
@@ -4383,7 +5175,7 @@
     </row>
     <row r="174" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G174" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="H174" t="s">
         <v>433</v>
@@ -4391,7 +5183,7 @@
     </row>
     <row r="175" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G175" t="s">
-        <v>163</v>
+        <v>270</v>
       </c>
       <c r="H175" t="s">
         <v>179</v>
@@ -4399,7 +5191,7 @@
     </row>
     <row r="176" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G176" t="s">
-        <v>384</v>
+        <v>264</v>
       </c>
       <c r="H176" t="s">
         <v>434</v>
@@ -4407,7 +5199,7 @@
     </row>
     <row r="177" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G177" t="s">
-        <v>385</v>
+        <v>159</v>
       </c>
       <c r="H177" t="s">
         <v>435</v>
@@ -4415,7 +5207,7 @@
     </row>
     <row r="178" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G178" t="s">
-        <v>386</v>
+        <v>197</v>
       </c>
       <c r="H178" t="s">
         <v>49</v>
@@ -4423,7 +5215,7 @@
     </row>
     <row r="179" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G179" t="s">
-        <v>387</v>
+        <v>111</v>
       </c>
       <c r="H179" t="s">
         <v>53</v>
@@ -4431,7 +5223,7 @@
     </row>
     <row r="180" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G180" t="s">
-        <v>388</v>
+        <v>287</v>
       </c>
       <c r="H180" t="s">
         <v>335</v>
@@ -4439,7 +5231,7 @@
     </row>
     <row r="181" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G181" t="s">
-        <v>389</v>
+        <v>108</v>
       </c>
       <c r="H181" t="s">
         <v>230</v>
@@ -4447,7 +5239,7 @@
     </row>
     <row r="182" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G182" t="s">
-        <v>113</v>
+        <v>366</v>
       </c>
       <c r="H182" t="s">
         <v>138</v>
@@ -4455,7 +5247,7 @@
     </row>
     <row r="183" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G183" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="H183" t="s">
         <v>436</v>
@@ -4463,7 +5255,7 @@
     </row>
     <row r="184" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G184" t="s">
-        <v>391</v>
+        <v>259</v>
       </c>
       <c r="H184" t="s">
         <v>437</v>
@@ -4471,7 +5263,7 @@
     </row>
     <row r="185" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G185" t="s">
-        <v>392</v>
+        <v>117</v>
       </c>
       <c r="H185" t="s">
         <v>438</v>
@@ -4479,7 +5271,7 @@
     </row>
     <row r="186" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G186" t="s">
-        <v>393</v>
+        <v>100</v>
       </c>
       <c r="H186" t="s">
         <v>439</v>
@@ -4487,7 +5279,7 @@
     </row>
     <row r="187" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G187" t="s">
-        <v>394</v>
+        <v>100</v>
       </c>
       <c r="H187" t="s">
         <v>184</v>
@@ -4495,7 +5287,7 @@
     </row>
     <row r="188" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G188" t="s">
-        <v>395</v>
+        <v>100</v>
       </c>
       <c r="H188" t="s">
         <v>128</v>
@@ -4503,7 +5295,7 @@
     </row>
     <row r="189" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G189" t="s">
-        <v>396</v>
+        <v>100</v>
       </c>
       <c r="H189" t="s">
         <v>57</v>
@@ -4511,7 +5303,7 @@
     </row>
     <row r="190" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G190" t="s">
-        <v>397</v>
+        <v>100</v>
       </c>
       <c r="H190" t="s">
         <v>49</v>
@@ -4519,7 +5311,7 @@
     </row>
     <row r="191" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G191" t="s">
-        <v>398</v>
+        <v>155</v>
       </c>
       <c r="H191" t="s">
         <v>440</v>
@@ -4527,7 +5319,7 @@
     </row>
     <row r="192" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G192" t="s">
-        <v>399</v>
+        <v>123</v>
       </c>
       <c r="H192" t="s">
         <v>441</v>
@@ -4535,7 +5327,7 @@
     </row>
     <row r="193" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G193" t="s">
-        <v>400</v>
+        <v>226</v>
       </c>
       <c r="H193" t="s">
         <v>53</v>
@@ -4543,7 +5335,7 @@
     </row>
     <row r="194" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G194" t="s">
-        <v>401</v>
+        <v>101</v>
       </c>
       <c r="H194" t="s">
         <v>442</v>
@@ -4551,7 +5343,7 @@
     </row>
     <row r="195" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G195" t="s">
-        <v>402</v>
+        <v>308</v>
       </c>
       <c r="H195" t="s">
         <v>324</v>
@@ -4559,7 +5351,7 @@
     </row>
     <row r="196" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G196" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="H196" t="s">
         <v>443</v>
@@ -4567,7 +5359,7 @@
     </row>
     <row r="197" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G197" t="s">
-        <v>404</v>
+        <v>416</v>
       </c>
       <c r="H197" t="s">
         <v>444</v>
@@ -4575,7 +5367,7 @@
     </row>
     <row r="198" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G198" t="s">
-        <v>405</v>
+        <v>288</v>
       </c>
       <c r="H198" t="s">
         <v>445</v>
@@ -4583,7 +5375,7 @@
     </row>
     <row r="199" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G199" t="s">
-        <v>406</v>
+        <v>109</v>
       </c>
       <c r="H199" t="s">
         <v>446</v>
@@ -4591,7 +5383,7 @@
     </row>
     <row r="200" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G200" t="s">
-        <v>407</v>
+        <v>244</v>
       </c>
       <c r="H200" t="s">
         <v>447</v>
@@ -4599,7 +5391,7 @@
     </row>
     <row r="201" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G201" t="s">
-        <v>408</v>
+        <v>365</v>
       </c>
       <c r="H201" t="s">
         <v>448</v>
@@ -4607,7 +5399,7 @@
     </row>
     <row r="202" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G202" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="H202" t="s">
         <v>449</v>
@@ -4615,7 +5407,7 @@
     </row>
     <row r="203" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G203" t="s">
-        <v>410</v>
+        <v>385</v>
       </c>
       <c r="H203" t="s">
         <v>232</v>
@@ -4623,7 +5415,7 @@
     </row>
     <row r="204" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G204" t="s">
-        <v>411</v>
+        <v>301</v>
       </c>
       <c r="H204" t="s">
         <v>450</v>
@@ -4631,7 +5423,7 @@
     </row>
     <row r="205" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G205" t="s">
-        <v>412</v>
+        <v>215</v>
       </c>
       <c r="H205" t="s">
         <v>230</v>
@@ -4639,7 +5431,7 @@
     </row>
     <row r="206" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G206" t="s">
-        <v>413</v>
+        <v>367</v>
       </c>
       <c r="H206" t="s">
         <v>451</v>
@@ -4647,7 +5439,7 @@
     </row>
     <row r="207" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G207" t="s">
-        <v>414</v>
+        <v>273</v>
       </c>
       <c r="H207" t="s">
         <v>49</v>
@@ -4655,7 +5447,7 @@
     </row>
     <row r="208" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G208" t="s">
-        <v>415</v>
+        <v>102</v>
       </c>
       <c r="H208" t="s">
         <v>452</v>
@@ -4663,7 +5455,7 @@
     </row>
     <row r="209" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G209" t="s">
-        <v>416</v>
+        <v>276</v>
       </c>
       <c r="H209" t="s">
         <v>453</v>
@@ -4671,13 +5463,16 @@
     </row>
     <row r="210" spans="7:8" x14ac:dyDescent="0.2">
       <c r="G210" t="s">
-        <v>417</v>
+        <v>392</v>
       </c>
       <c r="H210" t="s">
         <v>176</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="O2:O216">
+    <sortCondition ref="O1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added updates to fungi and cyano workup
</commit_message>
<xml_diff>
--- a/analyses/pronovo-2019/cyano-fungi-workup.xlsx
+++ b/analyses/pronovo-2019/cyano-fungi-workup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/meganduffy/Documents/git-repos/2017-etnp/analyses/pronovo-2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B72F28-0FF6-EF44-8623-451AA6135642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716492E8-91A6-7C45-9008-1BFEAE290EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="1" xr2:uid="{522D5D9C-FEE7-2041-BE17-7272E759D459}"/>
   </bookViews>
   <sheets>
     <sheet name="cyano dno + db peps tryptic" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="566">
   <si>
     <t>LASGLDAVTK</t>
   </si>
@@ -1708,6 +1708,30 @@
   </si>
   <si>
     <t>DLNALGFSDK</t>
+  </si>
+  <si>
+    <t>QLGLPADFVAK</t>
+  </si>
+  <si>
+    <t>AVAQLVEELAR</t>
+  </si>
+  <si>
+    <t>LTAHYCR</t>
+  </si>
+  <si>
+    <t>QDEVSQCWNNK</t>
+  </si>
+  <si>
+    <t>TEKPASDK</t>
+  </si>
+  <si>
+    <t>QAVSDDLLK</t>
+  </si>
+  <si>
+    <t>TLPPLNYNLVK</t>
+  </si>
+  <si>
+    <t>SLVTEHNK</t>
   </si>
 </sst>
 </file>
@@ -2070,10 +2094,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F8545A-13E4-384E-A901-CD63BD0C8560}">
-  <dimension ref="A1:N105"/>
+  <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M109" sqref="M109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2160,6 +2184,24 @@
       <c r="H2" t="s">
         <v>454</v>
       </c>
+      <c r="I2" t="s">
+        <v>558</v>
+      </c>
+      <c r="J2" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" t="s">
+        <v>560</v>
+      </c>
+      <c r="L2" t="s">
+        <v>561</v>
+      </c>
+      <c r="M2" t="s">
+        <v>562</v>
+      </c>
+      <c r="N2" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -2180,6 +2222,12 @@
       <c r="H3" t="s">
         <v>455</v>
       </c>
+      <c r="M3" t="s">
+        <v>563</v>
+      </c>
+      <c r="N3" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2197,6 +2245,12 @@
       <c r="H4" t="s">
         <v>456</v>
       </c>
+      <c r="M4" t="s">
+        <v>564</v>
+      </c>
+      <c r="N4" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -2214,6 +2268,12 @@
       <c r="H5" t="s">
         <v>457</v>
       </c>
+      <c r="M5" t="s">
+        <v>565</v>
+      </c>
+      <c r="N5" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -2228,6 +2288,9 @@
       <c r="H6" t="s">
         <v>458</v>
       </c>
+      <c r="N6" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
@@ -2242,6 +2305,9 @@
       <c r="H7" t="s">
         <v>459</v>
       </c>
+      <c r="N7" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
@@ -2253,6 +2319,9 @@
       <c r="H8" t="s">
         <v>460</v>
       </c>
+      <c r="N8" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G9" s="2" t="s">
@@ -2261,6 +2330,9 @@
       <c r="H9" t="s">
         <v>461</v>
       </c>
+      <c r="N9" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G10" s="2" t="s">
@@ -2269,6 +2341,9 @@
       <c r="H10" t="s">
         <v>462</v>
       </c>
+      <c r="N10" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G11" s="2" t="s">
@@ -2277,6 +2352,9 @@
       <c r="H11" t="s">
         <v>463</v>
       </c>
+      <c r="N11" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G12" s="2" t="s">
@@ -2285,6 +2363,9 @@
       <c r="H12" t="s">
         <v>464</v>
       </c>
+      <c r="N12" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G13" s="2" t="s">
@@ -2293,6 +2374,9 @@
       <c r="H13" t="s">
         <v>465</v>
       </c>
+      <c r="N13" t="s">
+        <v>465</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G14" s="2" t="s">
@@ -2301,6 +2385,9 @@
       <c r="H14" t="s">
         <v>466</v>
       </c>
+      <c r="N14" t="s">
+        <v>466</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G15" s="2" t="s">
@@ -2309,6 +2396,9 @@
       <c r="H15" t="s">
         <v>467</v>
       </c>
+      <c r="N15" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="G16" s="2" t="s">
@@ -2317,465 +2407,775 @@
       <c r="H16" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="17" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H17" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="18" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="H18" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="19" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G19" s="2" t="s">
         <v>16</v>
       </c>
       <c r="H19" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="20" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="20" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="H20" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="21" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="21" spans="7:14" x14ac:dyDescent="0.2">
       <c r="G21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="H21" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="22" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N21" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H22" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="23" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N22" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="23" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H23" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="24" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N23" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="24" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H24" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="25" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N24" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="25" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H25" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="26" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N25" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="26" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="27" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N26" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="27" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N27" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="28" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N28" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="29" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N29" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="30" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="31" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N30" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="31" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="32" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="N31" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="32" spans="7:14" x14ac:dyDescent="0.2">
       <c r="H32" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="33" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N32" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="33" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H33" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="34" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N33" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="34" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H34" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="35" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N34" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="35" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H35" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="36" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N35" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="36" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H36" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="37" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N36" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="37" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H37" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="38" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N37" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="38" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H38" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="39" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N38" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="39" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H39" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="40" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N39" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="40" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H40" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="41" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N40" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="41" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H41" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="42" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N41" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="42" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H42" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="43" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N42" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="43" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H43" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="44" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N43" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="44" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H44" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="45" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N44" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="45" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H45" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="46" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N45" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="46" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H46" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="47" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N46" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="47" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H47" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="48" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N47" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="48" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H48" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="49" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N48" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H49" t="s">
         <v>501</v>
       </c>
-    </row>
-    <row r="50" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N49" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="50" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H50" t="s">
         <v>502</v>
       </c>
-    </row>
-    <row r="51" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N50" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="51" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H51" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="52" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N51" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="52" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H52" t="s">
         <v>504</v>
       </c>
-    </row>
-    <row r="53" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N52" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="53" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H53" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="54" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N53" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="54" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H54" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="55" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N54" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="55" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H55" t="s">
         <v>507</v>
       </c>
-    </row>
-    <row r="56" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N55" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="56" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H56" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="57" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N56" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="57" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H57" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="58" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N57" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="58" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H58" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="59" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N58" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="59" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H59" t="s">
         <v>511</v>
       </c>
-    </row>
-    <row r="60" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N59" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="60" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H60" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="61" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N60" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="61" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H61" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="62" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N61" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="62" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H62" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="63" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N62" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="63" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H63" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="64" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N63" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="64" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H64" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="65" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N64" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="65" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H65" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="66" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N65" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="66" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H66" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="67" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N66" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="67" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H67" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="68" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N67" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="68" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H68" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="69" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N68" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="69" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H69" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="70" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N69" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="70" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H70" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="71" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N70" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="71" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H71" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="72" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N71" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="72" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H72" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="73" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N72" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="73" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H73" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="74" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N73" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="74" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H74" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="75" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N74" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="75" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H75" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="76" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N75" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="76" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H76" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="77" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N76" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="77" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H77" t="s">
         <v>529</v>
       </c>
-    </row>
-    <row r="78" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N77" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="78" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H78" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="79" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N78" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="79" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H79" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="80" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N79" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="80" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H80" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="81" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N80" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="81" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H81" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="82" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N81" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="82" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H82" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="83" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N82" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="83" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H83" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="84" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N83" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="84" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H84" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="85" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N84" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="85" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H85" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="86" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N85" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="86" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H86" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="87" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N86" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="87" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H87" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="88" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N87" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="88" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H88" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="89" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N88" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="89" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H89" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="90" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N89" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="90" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H90" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="91" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N90" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="91" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H91" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="92" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N91" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="92" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H92" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="93" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N92" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="93" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H93" t="s">
         <v>545</v>
       </c>
-    </row>
-    <row r="94" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N93" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="94" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H94" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="95" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N94" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="95" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H95" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="96" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N95" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="96" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H96" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="97" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N96" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="97" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H97" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="98" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N97" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="98" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H98" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="99" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N98" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="99" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H99" t="s">
         <v>551</v>
       </c>
-    </row>
-    <row r="100" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N99" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="100" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H100" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="101" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N100" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="101" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H101" t="s">
         <v>553</v>
       </c>
-    </row>
-    <row r="102" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N101" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="102" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H102" t="s">
         <v>554</v>
       </c>
-    </row>
-    <row r="103" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N102" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="103" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H103" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="104" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N103" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="104" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H104" t="s">
         <v>556</v>
       </c>
-    </row>
-    <row r="105" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="N104" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="105" spans="8:14" x14ac:dyDescent="0.2">
       <c r="H105" t="s">
         <v>557</v>
+      </c>
+      <c r="N105" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="106" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N106" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="107" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N107" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="108" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N108" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="109" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N109" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="110" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N110" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="111" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N111" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="112" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="N112" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="113" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N113" t="s">
+        <v>565</v>
       </c>
     </row>
   </sheetData>
@@ -2791,7 +3191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE39D6E-ADCE-C54E-86E3-C5932C98575B}">
   <dimension ref="A1:P210"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>